<commit_message>
re-estimated health and wellbeing variables
</commit_message>
<xml_diff>
--- a/input/reg_health_mental.xlsx
+++ b/input/reg_health_mental.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\andy_local\SimPaths project files\SimPaths\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06CAAE0F-C79D-450E-ACEA-9E2AF93D6301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D179F5-C628-4575-84B9-9FD17F5D5FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="27000" windowHeight="14100" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="27000" windowHeight="14100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="2" r:id="rId1"/>
@@ -18,11 +18,11 @@
     <sheet name="UK_HM1_C" sheetId="7" r:id="rId3"/>
     <sheet name="UK_HM2_Males_C" sheetId="8" r:id="rId4"/>
     <sheet name="UK_HM2_Females_C" sheetId="9" r:id="rId5"/>
-    <sheet name="UK_HM1_L" sheetId="13" r:id="rId6"/>
-    <sheet name="UK_HM2_Males_L" sheetId="14" r:id="rId7"/>
-    <sheet name="UK_HM2_Females_L" sheetId="15" r:id="rId8"/>
+    <sheet name="UK_HM1_L" sheetId="16" r:id="rId6"/>
+    <sheet name="UK_HM2_Males_L" sheetId="17" r:id="rId7"/>
+    <sheet name="UK_HM2_Females_L" sheetId="18" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -4326,7 +4326,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F83C27E0-FA2B-440E-9BE2-866FFC98D161}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4757,14 +4757,15 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB3203A6-DA5F-4B51-8074-D30044B6B769}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFA65DFE-C60F-4D4D-8008-9FC7A3FF9E6E}">
   <dimension ref="A1:AF31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.42578125" style="8"/>
+    <col min="1" max="1" width="30.7109375" style="8" customWidth="1"/>
+    <col min="2" max="16384" width="11.42578125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.25">
@@ -4870,97 +4871,97 @@
         <v>34</v>
       </c>
       <c r="B2" s="8">
-        <v>0.18952543247051801</v>
+        <v>0.21548707218562399</v>
       </c>
       <c r="C2" s="8">
-        <v>1.6610316565265201E-3</v>
+        <v>1.25374527274403E-3</v>
       </c>
       <c r="D2" s="8">
-        <v>-2.2452002236969702E-5</v>
+        <v>-2.4394791244791601E-5</v>
       </c>
       <c r="E2" s="8">
-        <v>4.3007103477225698E-4</v>
+        <v>2.93026348970292E-4</v>
       </c>
       <c r="F2" s="8">
-        <v>1.18020264249732E-4</v>
+        <v>9.9212587927633903E-5</v>
       </c>
       <c r="G2" s="8">
-        <v>2.62284068317879E-5</v>
+        <v>1.15170236347298E-5</v>
       </c>
       <c r="H2" s="8">
-        <v>7.3528749218372406E-5</v>
+        <v>3.5957899469002198E-5</v>
       </c>
       <c r="I2" s="8">
-        <v>-1.02248353012786E-4</v>
+        <v>-3.3624695957226197E-5</v>
       </c>
       <c r="J2" s="8">
-        <v>-1.16399598403884E-4</v>
+        <v>-5.6980063456238399E-5</v>
       </c>
       <c r="K2" s="8">
-        <v>-9.4741592403615603E-5</v>
+        <v>-3.3140607190495601E-5</v>
       </c>
       <c r="L2" s="8">
-        <v>-5.4350626647645903E-5</v>
+        <v>-3.6026752548505101E-6</v>
       </c>
       <c r="M2" s="8">
-        <v>-1.03792828150084E-5</v>
+        <v>-5.8135899523151103E-6</v>
       </c>
       <c r="N2" s="8">
-        <v>-2.63902686176086E-6</v>
+        <v>2.6292523201600701E-5</v>
       </c>
       <c r="O2" s="8">
-        <v>-9.9363622412932599E-5</v>
+        <v>-3.1916735306552297E-5</v>
       </c>
       <c r="P2" s="8">
-        <v>-5.9207400570414001E-5</v>
+        <v>-1.3920141205489E-5</v>
       </c>
       <c r="Q2" s="8">
-        <v>1.8828056144282501E-5</v>
+        <v>7.0784726374946501E-6</v>
       </c>
       <c r="R2" s="8">
-        <v>-1.1829564444302599E-4</v>
+        <v>-5.1913341417064199E-5</v>
       </c>
       <c r="S2" s="8">
-        <v>-3.8159597474569099E-5</v>
+        <v>9.0654499959562297E-7</v>
       </c>
       <c r="T2" s="8">
-        <v>-2.1242328967870799E-4</v>
+        <v>-1.7042693690025399E-4</v>
       </c>
       <c r="U2" s="8">
-        <v>-1.28929979797121E-4</v>
+        <v>-1.06933575513096E-4</v>
       </c>
       <c r="V2" s="8">
-        <v>1.1912362644709499E-5</v>
+        <v>1.91159661513898E-6</v>
       </c>
       <c r="W2" s="8">
-        <v>1.6869150462134699E-4</v>
+        <v>1.17173090250836E-4</v>
       </c>
       <c r="X2" s="8">
-        <v>3.5420281375932698E-4</v>
+        <v>2.5661305439669699E-4</v>
       </c>
       <c r="Y2" s="8">
-        <v>-3.2704333110136102E-4</v>
+        <v>-2.2776585886313499E-4</v>
       </c>
       <c r="Z2" s="8">
-        <v>2.5770534110842701E-5</v>
+        <v>1.7418917226673301E-5</v>
       </c>
       <c r="AA2" s="8">
-        <v>4.9960856219291698E-5</v>
+        <v>3.8277125207519503E-5</v>
       </c>
       <c r="AB2" s="8">
-        <v>-5.9271209308084304E-7</v>
+        <v>-4.4866372998640298E-7</v>
       </c>
       <c r="AC2" s="8">
-        <v>1.9537367433311E-7</v>
+        <v>-2.0624941559523401E-6</v>
       </c>
       <c r="AD2" s="8">
-        <v>-2.2478727004080199E-7</v>
+        <v>-9.5378344862199601E-8</v>
       </c>
       <c r="AE2" s="8">
-        <v>3.4765388771384202E-5</v>
+        <v>3.56806776970703E-5</v>
       </c>
       <c r="AF2" s="8">
-        <v>-2.4542698855680098E-3</v>
+        <v>-1.8331472171509999E-3</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
@@ -4968,97 +4969,97 @@
         <v>35</v>
       </c>
       <c r="B3" s="8">
-        <v>-0.32651727558283</v>
+        <v>-0.32346937051376501</v>
       </c>
       <c r="C3" s="8">
-        <v>-2.2452002236969702E-5</v>
+        <v>-2.4394791244791601E-5</v>
       </c>
       <c r="D3" s="8">
-        <v>2.6465598070934898E-3</v>
+        <v>1.9635982758812302E-3</v>
       </c>
       <c r="E3" s="8">
-        <v>-2.56272857333913E-5</v>
+        <v>-6.0324293385774998E-5</v>
       </c>
       <c r="F3" s="8">
-        <v>3.0798305403642102E-4</v>
+        <v>2.1159106935589601E-4</v>
       </c>
       <c r="G3" s="8">
-        <v>1.41750967245019E-4</v>
+        <v>5.6513115539546002E-5</v>
       </c>
       <c r="H3" s="8">
-        <v>3.9896911344732E-4</v>
+        <v>2.4743138940388798E-4</v>
       </c>
       <c r="I3" s="8">
-        <v>-5.2016872557828495E-4</v>
+        <v>-3.20603147445324E-4</v>
       </c>
       <c r="J3" s="8">
-        <v>-7.1231702273110396E-4</v>
+        <v>-4.4830984460138702E-4</v>
       </c>
       <c r="K3" s="8">
-        <v>-4.14376837020491E-4</v>
+        <v>-2.2976425546571001E-4</v>
       </c>
       <c r="L3" s="8">
-        <v>-5.5623871038439098E-4</v>
+        <v>-3.5132083779069502E-4</v>
       </c>
       <c r="M3" s="8">
-        <v>-6.7266191752578502E-4</v>
+        <v>-4.6152293938123498E-4</v>
       </c>
       <c r="N3" s="8">
-        <v>-5.2397664131760004E-4</v>
+        <v>-3.5275221770223402E-4</v>
       </c>
       <c r="O3" s="8">
-        <v>-5.5506112148713397E-4</v>
+        <v>-3.5054121855327601E-4</v>
       </c>
       <c r="P3" s="8">
-        <v>-6.0942872218548499E-4</v>
+        <v>-3.9440505676415898E-4</v>
       </c>
       <c r="Q3" s="8">
-        <v>-8.0115066736729905E-4</v>
+        <v>-6.1019892780987499E-4</v>
       </c>
       <c r="R3" s="8">
-        <v>-6.6449482002627297E-4</v>
+        <v>-4.2531167881112899E-4</v>
       </c>
       <c r="S3" s="8">
-        <v>-8.4574341081580697E-4</v>
+        <v>-5.4483268097545504E-4</v>
       </c>
       <c r="T3" s="8">
-        <v>-2.44476234846575E-4</v>
+        <v>-1.5726936471822299E-4</v>
       </c>
       <c r="U3" s="8">
-        <v>2.5523831405678999E-5</v>
+        <v>-1.7628097143113999E-5</v>
       </c>
       <c r="V3" s="8">
-        <v>-2.6638431963693399E-4</v>
+        <v>-2.35190709147246E-4</v>
       </c>
       <c r="W3" s="8">
-        <v>-4.60062817506805E-4</v>
+        <v>-3.9707618216626098E-4</v>
       </c>
       <c r="X3" s="8">
-        <v>-5.7627961049298404E-4</v>
+        <v>-4.6418451004554001E-4</v>
       </c>
       <c r="Y3" s="8">
-        <v>8.5721246069600998E-4</v>
+        <v>6.2970740391318899E-4</v>
       </c>
       <c r="Z3" s="8">
-        <v>-2.4265473526926501E-5</v>
+        <v>-2.1762751755166099E-5</v>
       </c>
       <c r="AA3" s="8">
-        <v>-2.8996706449829501E-5</v>
+        <v>-2.26315833790098E-5</v>
       </c>
       <c r="AB3" s="8">
-        <v>1.4044594011223399E-7</v>
+        <v>1.12089594352502E-7</v>
       </c>
       <c r="AC3" s="8">
-        <v>2.8337035697823298E-5</v>
+        <v>1.7858610406278699E-5</v>
       </c>
       <c r="AD3" s="8">
-        <v>-7.3764160587729402E-6</v>
+        <v>-5.1376684707118898E-6</v>
       </c>
       <c r="AE3" s="8">
-        <v>2.4381918286106602E-5</v>
+        <v>3.2141074307096401E-5</v>
       </c>
       <c r="AF3" s="8">
-        <v>2.7313052606342701E-5</v>
+        <v>1.3314311295563701E-4</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
@@ -5066,97 +5067,97 @@
         <v>21</v>
       </c>
       <c r="B4" s="8">
-        <v>0.22590766188670799</v>
+        <v>0.17451599165659101</v>
       </c>
       <c r="C4" s="8">
-        <v>4.3007103477225698E-4</v>
+        <v>2.93026348970292E-4</v>
       </c>
       <c r="D4" s="8">
-        <v>-2.56272857333913E-5</v>
+        <v>-6.0324293385774998E-5</v>
       </c>
       <c r="E4" s="8">
-        <v>4.2488655663507199E-3</v>
+        <v>3.21459864438333E-3</v>
       </c>
       <c r="F4" s="8">
-        <v>3.3026037937025301E-4</v>
+        <v>2.6698399105957901E-4</v>
       </c>
       <c r="G4" s="8">
-        <v>-1.3915370431770199E-4</v>
+        <v>-1.10100194163848E-4</v>
       </c>
       <c r="H4" s="8">
-        <v>1.1683660262775099E-5</v>
+        <v>-1.1781781138685E-5</v>
       </c>
       <c r="I4" s="8">
-        <v>2.8994594986839802E-4</v>
+        <v>2.3294998669425401E-4</v>
       </c>
       <c r="J4" s="8">
-        <v>3.7760747091908001E-4</v>
+        <v>2.0684718294199599E-4</v>
       </c>
       <c r="K4" s="8">
-        <v>2.4763768093902E-4</v>
+        <v>2.3005346791499999E-4</v>
       </c>
       <c r="L4" s="8">
-        <v>4.3657464900601198E-4</v>
+        <v>3.11404916713212E-4</v>
       </c>
       <c r="M4" s="8">
-        <v>5.8783018712168101E-4</v>
+        <v>3.4570204999660303E-4</v>
       </c>
       <c r="N4" s="8">
-        <v>4.4859149736028699E-4</v>
+        <v>2.9448154059105697E-4</v>
       </c>
       <c r="O4" s="8">
-        <v>4.0677706934950599E-4</v>
+        <v>2.6739695011598902E-4</v>
       </c>
       <c r="P4" s="8">
-        <v>4.5665169764451001E-4</v>
+        <v>3.22114963046491E-4</v>
       </c>
       <c r="Q4" s="8">
-        <v>7.7475942359961001E-4</v>
+        <v>6.5435228250584204E-4</v>
       </c>
       <c r="R4" s="8">
-        <v>3.6196407345823E-4</v>
+        <v>1.8643456883649201E-4</v>
       </c>
       <c r="S4" s="8">
-        <v>2.89766996693161E-4</v>
+        <v>1.5896051790660899E-4</v>
       </c>
       <c r="T4" s="8">
-        <v>-2.0946537737323801E-4</v>
+        <v>-2.12827260295729E-4</v>
       </c>
       <c r="U4" s="8">
-        <v>1.9055926048402099E-4</v>
+        <v>1.3180405573850801E-4</v>
       </c>
       <c r="V4" s="8">
-        <v>3.2630455617718398E-4</v>
+        <v>2.8501890220112902E-4</v>
       </c>
       <c r="W4" s="8">
-        <v>4.2819227027188499E-4</v>
+        <v>3.6482712876218898E-4</v>
       </c>
       <c r="X4" s="8">
-        <v>4.2022039204532298E-4</v>
+        <v>3.4535045012430802E-4</v>
       </c>
       <c r="Y4" s="8">
-        <v>-1.89962332863713E-4</v>
+        <v>-2.0417905428785099E-4</v>
       </c>
       <c r="Z4" s="8">
-        <v>-9.91938982984867E-6</v>
+        <v>1.7149527807957399E-6</v>
       </c>
       <c r="AA4" s="8">
-        <v>2.1523857111346501E-4</v>
+        <v>1.68765660797707E-4</v>
       </c>
       <c r="AB4" s="8">
-        <v>-1.8168299274073099E-6</v>
+        <v>-1.42675270740487E-6</v>
       </c>
       <c r="AC4" s="8">
-        <v>-1.84771376259494E-5</v>
+        <v>-1.3072422088211801E-5</v>
       </c>
       <c r="AD4" s="8">
-        <v>-7.7207431865631299E-7</v>
+        <v>-5.4949633685124295E-7</v>
       </c>
       <c r="AE4" s="8">
-        <v>5.6212547344424101E-5</v>
+        <v>4.0434918179314501E-5</v>
       </c>
       <c r="AF4" s="8">
-        <v>-6.9135954020958096E-3</v>
+        <v>-5.4429747032758297E-3</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
@@ -5164,97 +5165,97 @@
         <v>22</v>
       </c>
       <c r="B5" s="8">
-        <v>0.19469523141464901</v>
+        <v>0.194320104787508</v>
       </c>
       <c r="C5" s="8">
-        <v>1.18020264249732E-4</v>
+        <v>9.9212587927633903E-5</v>
       </c>
       <c r="D5" s="8">
-        <v>3.0798305403642102E-4</v>
+        <v>2.1159106935589601E-4</v>
       </c>
       <c r="E5" s="8">
-        <v>3.3026037937025301E-4</v>
+        <v>2.6698399105957901E-4</v>
       </c>
       <c r="F5" s="8">
-        <v>2.9801614049548698E-3</v>
+        <v>2.4386117152754298E-3</v>
       </c>
       <c r="G5" s="8">
-        <v>-8.4580165128951698E-5</v>
+        <v>-5.1872043583856699E-5</v>
       </c>
       <c r="H5" s="8">
-        <v>-5.5944857527943103E-5</v>
+        <v>-2.6790636926445599E-5</v>
       </c>
       <c r="I5" s="8">
-        <v>1.9704315613348899E-4</v>
+        <v>1.4147586472680501E-4</v>
       </c>
       <c r="J5" s="8">
-        <v>-1.95094305549042E-4</v>
+        <v>-1.26285813992448E-4</v>
       </c>
       <c r="K5" s="8">
-        <v>-1.3353489737905601E-4</v>
+        <v>-5.5232721570482302E-5</v>
       </c>
       <c r="L5" s="8">
-        <v>-1.5390064258914599E-5</v>
+        <v>-1.07577635217511E-5</v>
       </c>
       <c r="M5" s="8">
-        <v>8.0183589488082006E-5</v>
+        <v>8.6543257663103203E-5</v>
       </c>
       <c r="N5" s="8">
-        <v>-4.6229899146876597E-5</v>
+        <v>2.2338614595099699E-5</v>
       </c>
       <c r="O5" s="8">
-        <v>-1.03273264004224E-4</v>
+        <v>-4.2191481593052299E-5</v>
       </c>
       <c r="P5" s="8">
-        <v>-9.8782636777001602E-5</v>
+        <v>-4.8724689555940298E-5</v>
       </c>
       <c r="Q5" s="8">
-        <v>1.9345962453120899E-4</v>
+        <v>1.5903834510351401E-4</v>
       </c>
       <c r="R5" s="8">
-        <v>-2.7882665247920199E-4</v>
+        <v>-1.48122627785236E-4</v>
       </c>
       <c r="S5" s="8">
-        <v>-2.7584955475909499E-4</v>
+        <v>-1.61917970891495E-4</v>
       </c>
       <c r="T5" s="8">
-        <v>-3.9731775296312199E-5</v>
+        <v>-2.7993404341663698E-5</v>
       </c>
       <c r="U5" s="8">
-        <v>5.81332560639315E-5</v>
+        <v>3.1765119593700298E-5</v>
       </c>
       <c r="V5" s="8">
-        <v>1.7026975078599099E-4</v>
+        <v>1.1021180503455699E-4</v>
       </c>
       <c r="W5" s="8">
-        <v>2.1032483690185401E-4</v>
+        <v>1.75757031507802E-4</v>
       </c>
       <c r="X5" s="8">
-        <v>2.7891371757865702E-4</v>
+        <v>2.32170272959106E-4</v>
       </c>
       <c r="Y5" s="8">
-        <v>-6.20921941204557E-5</v>
+        <v>-1.03556653835802E-4</v>
       </c>
       <c r="Z5" s="8">
-        <v>7.8306114194152597E-6</v>
+        <v>3.1585411834741901E-6</v>
       </c>
       <c r="AA5" s="8">
-        <v>2.8670363005618002E-5</v>
+        <v>2.2092207183286601E-5</v>
       </c>
       <c r="AB5" s="8">
-        <v>-4.47720382063782E-7</v>
+        <v>-3.50618630472197E-7</v>
       </c>
       <c r="AC5" s="8">
-        <v>-9.4755087277608297E-6</v>
+        <v>-9.7764234897121507E-6</v>
       </c>
       <c r="AD5" s="8">
-        <v>3.8557142933592896E-6</v>
+        <v>3.3160001429759501E-6</v>
       </c>
       <c r="AE5" s="8">
-        <v>2.2053885031994599E-4</v>
+        <v>1.58240065566467E-4</v>
       </c>
       <c r="AF5" s="8">
-        <v>-1.2890159632446599E-3</v>
+        <v>-9.6146032241205097E-4</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
@@ -5262,97 +5263,97 @@
         <v>19</v>
       </c>
       <c r="B6" s="8">
-        <v>2.5458165929038001E-2</v>
+        <v>4.6885140752195298E-2</v>
       </c>
       <c r="C6" s="8">
-        <v>2.62284068317879E-5</v>
+        <v>1.15170236347298E-5</v>
       </c>
       <c r="D6" s="8">
-        <v>1.41750967245019E-4</v>
+        <v>5.6513115539546002E-5</v>
       </c>
       <c r="E6" s="8">
-        <v>-1.3915370431770199E-4</v>
+        <v>-1.10100194163848E-4</v>
       </c>
       <c r="F6" s="8">
-        <v>-8.4580165128951698E-5</v>
+        <v>-5.1872043583856699E-5</v>
       </c>
       <c r="G6" s="8">
-        <v>1.84660986008461E-3</v>
+        <v>1.4954878314086301E-3</v>
       </c>
       <c r="H6" s="8">
-        <v>1.3273442897852501E-3</v>
+        <v>1.0901954247889E-3</v>
       </c>
       <c r="I6" s="8">
-        <v>-6.6207627846813499E-4</v>
+        <v>-5.1403577458328101E-4</v>
       </c>
       <c r="J6" s="8">
-        <v>-6.0221942485362903E-4</v>
+        <v>-4.5895451737053901E-4</v>
       </c>
       <c r="K6" s="8">
-        <v>-5.2754163679131398E-4</v>
+        <v>-3.8567926345713999E-4</v>
       </c>
       <c r="L6" s="8">
-        <v>-6.8903916357526695E-4</v>
+        <v>-5.2028759380593999E-4</v>
       </c>
       <c r="M6" s="8">
-        <v>-7.8366353885107301E-4</v>
+        <v>-5.6973404853032604E-4</v>
       </c>
       <c r="N6" s="8">
-        <v>-5.2772343135743102E-4</v>
+        <v>-4.2316898859286298E-4</v>
       </c>
       <c r="O6" s="8">
-        <v>-5.4675858160080002E-4</v>
+        <v>-4.2519474578210702E-4</v>
       </c>
       <c r="P6" s="8">
-        <v>-5.5763362677569101E-4</v>
+        <v>-4.5651480665931599E-4</v>
       </c>
       <c r="Q6" s="8">
-        <v>-5.3898399279217696E-4</v>
+        <v>-3.9053190811033298E-4</v>
       </c>
       <c r="R6" s="8">
-        <v>-4.1045282850515598E-4</v>
+        <v>-3.40608746747858E-4</v>
       </c>
       <c r="S6" s="8">
-        <v>-5.0834864668053198E-4</v>
+        <v>-3.8424220541903001E-4</v>
       </c>
       <c r="T6" s="8">
-        <v>-2.2342855962618501E-4</v>
+        <v>-1.90048164124522E-4</v>
       </c>
       <c r="U6" s="8">
-        <v>-1.04632177757973E-4</v>
+        <v>-8.0763238596518396E-5</v>
       </c>
       <c r="V6" s="8">
-        <v>-4.2819949118650899E-5</v>
+        <v>-3.1488974456466399E-5</v>
       </c>
       <c r="W6" s="8">
-        <v>1.26938335667565E-5</v>
+        <v>2.8661231781060401E-5</v>
       </c>
       <c r="X6" s="8">
-        <v>2.9569886621756702E-4</v>
+        <v>2.5053514890331402E-4</v>
       </c>
       <c r="Y6" s="8">
-        <v>-1.9854278345841201E-4</v>
+        <v>-1.3187972664026299E-4</v>
       </c>
       <c r="Z6" s="8">
-        <v>2.4286068127837401E-5</v>
+        <v>2.04754450575988E-5</v>
       </c>
       <c r="AA6" s="8">
-        <v>-1.311447909988E-5</v>
+        <v>-3.2191950471297599E-6</v>
       </c>
       <c r="AB6" s="8">
-        <v>7.7556325408841003E-8</v>
+        <v>-2.4461453760613501E-9</v>
       </c>
       <c r="AC6" s="8">
-        <v>3.2520195486707897E-5</v>
+        <v>2.1714595934536899E-5</v>
       </c>
       <c r="AD6" s="8">
-        <v>6.8154745404337501E-6</v>
+        <v>5.0993407326699696E-6</v>
       </c>
       <c r="AE6" s="8">
-        <v>-5.2204729394408401E-5</v>
+        <v>-3.59681661507263E-5</v>
       </c>
       <c r="AF6" s="8">
-        <v>-1.3619116532863601E-3</v>
+        <v>-1.2169697293377901E-3</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
@@ -5360,97 +5361,97 @@
         <v>20</v>
       </c>
       <c r="B7" s="8">
-        <v>2.7384835178281702E-2</v>
+        <v>7.0931200431388702E-2</v>
       </c>
       <c r="C7" s="8">
-        <v>7.3528749218372406E-5</v>
+        <v>3.5957899469002198E-5</v>
       </c>
       <c r="D7" s="8">
-        <v>3.9896911344732E-4</v>
+        <v>2.4743138940388798E-4</v>
       </c>
       <c r="E7" s="8">
-        <v>1.1683660262775099E-5</v>
+        <v>-1.1781781138685E-5</v>
       </c>
       <c r="F7" s="8">
-        <v>-5.5944857527943103E-5</v>
+        <v>-2.6790636926445599E-5</v>
       </c>
       <c r="G7" s="8">
-        <v>1.3273442897852501E-3</v>
+        <v>1.0901954247889E-3</v>
       </c>
       <c r="H7" s="8">
-        <v>3.6063625311437701E-3</v>
+        <v>2.8726830479096901E-3</v>
       </c>
       <c r="I7" s="8">
-        <v>-6.6509592731976296E-4</v>
+        <v>-5.74949288102367E-4</v>
       </c>
       <c r="J7" s="8">
-        <v>-3.7353833085214302E-4</v>
+        <v>-3.70604266139672E-4</v>
       </c>
       <c r="K7" s="8">
-        <v>-3.8067009212457397E-4</v>
+        <v>-3.33217203581994E-4</v>
       </c>
       <c r="L7" s="8">
-        <v>-4.8632167939121002E-4</v>
+        <v>-4.6890013442667E-4</v>
       </c>
       <c r="M7" s="8">
-        <v>-6.8660318474704398E-4</v>
+        <v>-5.8122075101469902E-4</v>
       </c>
       <c r="N7" s="8">
-        <v>-4.86744667460091E-4</v>
+        <v>-4.4318131596151499E-4</v>
       </c>
       <c r="O7" s="8">
-        <v>-3.8040131403236602E-4</v>
+        <v>-3.4991666551239397E-4</v>
       </c>
       <c r="P7" s="8">
-        <v>-3.1228086118793603E-4</v>
+        <v>-3.4582868039585799E-4</v>
       </c>
       <c r="Q7" s="8">
-        <v>-4.3244966480001702E-4</v>
+        <v>-4.19041373455933E-4</v>
       </c>
       <c r="R7" s="8">
-        <v>-1.5628089169628399E-4</v>
+        <v>-1.8354713762818101E-4</v>
       </c>
       <c r="S7" s="8">
-        <v>-7.3661028076579197E-4</v>
+        <v>-6.1258261392858502E-4</v>
       </c>
       <c r="T7" s="8">
-        <v>-1.3655058035892299E-4</v>
+        <v>-1.2664173552619299E-4</v>
       </c>
       <c r="U7" s="8">
-        <v>-3.9061091234269703E-5</v>
+        <v>-1.3357685690987399E-5</v>
       </c>
       <c r="V7" s="8">
-        <v>1.36876311242743E-4</v>
+        <v>1.4670503203129001E-4</v>
       </c>
       <c r="W7" s="8">
-        <v>2.8534020577091802E-4</v>
+        <v>3.0335887083627803E-4</v>
       </c>
       <c r="X7" s="8">
-        <v>6.5824210999291003E-4</v>
+        <v>5.6827631859252003E-4</v>
       </c>
       <c r="Y7" s="8">
-        <v>-1.26608064496211E-4</v>
+        <v>-9.2684217219427404E-5</v>
       </c>
       <c r="Z7" s="8">
-        <v>5.4445328476127101E-5</v>
+        <v>4.91463903769168E-5</v>
       </c>
       <c r="AA7" s="8">
-        <v>2.2964596690976501E-5</v>
+        <v>1.36824618717904E-5</v>
       </c>
       <c r="AB7" s="8">
-        <v>-4.59798533174453E-7</v>
+        <v>-3.2391900034712001E-7</v>
       </c>
       <c r="AC7" s="8">
-        <v>2.7340167579836E-5</v>
+        <v>1.5800251116395101E-5</v>
       </c>
       <c r="AD7" s="8">
-        <v>8.6260049450565798E-6</v>
+        <v>7.1121667669341403E-6</v>
       </c>
       <c r="AE7" s="8">
-        <v>8.1975869074248398E-5</v>
+        <v>1.9493443158649301E-5</v>
       </c>
       <c r="AF7" s="8">
-        <v>-2.9328679580843601E-3</v>
+        <v>-2.16736343368281E-3</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
@@ -5458,97 +5459,97 @@
         <v>23</v>
       </c>
       <c r="B8" s="8">
-        <v>5.8772725881794897E-3</v>
+        <v>-1.3656295529287399E-2</v>
       </c>
       <c r="C8" s="8">
-        <v>-1.02248353012786E-4</v>
+        <v>-3.3624695957226197E-5</v>
       </c>
       <c r="D8" s="8">
-        <v>-5.2016872557828495E-4</v>
+        <v>-3.20603147445324E-4</v>
       </c>
       <c r="E8" s="8">
-        <v>2.8994594986839802E-4</v>
+        <v>2.3294998669425401E-4</v>
       </c>
       <c r="F8" s="8">
-        <v>1.9704315613348899E-4</v>
+        <v>1.4147586472680501E-4</v>
       </c>
       <c r="G8" s="8">
-        <v>-6.6207627846813499E-4</v>
+        <v>-5.1403577458328101E-4</v>
       </c>
       <c r="H8" s="8">
-        <v>-6.6509592731976296E-4</v>
+        <v>-5.74949288102367E-4</v>
       </c>
       <c r="I8" s="8">
-        <v>1.2910651726133799E-2</v>
+        <v>1.00676309778432E-2</v>
       </c>
       <c r="J8" s="8">
-        <v>4.91706013151852E-3</v>
+        <v>3.6743190023038599E-3</v>
       </c>
       <c r="K8" s="8">
-        <v>4.8906783378952802E-3</v>
+        <v>3.6653930960894999E-3</v>
       </c>
       <c r="L8" s="8">
-        <v>4.9296372906032998E-3</v>
+        <v>3.6962821497148199E-3</v>
       </c>
       <c r="M8" s="8">
-        <v>4.9603592623371599E-3</v>
+        <v>3.7101042049958901E-3</v>
       </c>
       <c r="N8" s="8">
-        <v>4.8257283805805398E-3</v>
+        <v>3.6277547096365201E-3</v>
       </c>
       <c r="O8" s="8">
-        <v>4.8206825441132802E-3</v>
+        <v>3.61994904942705E-3</v>
       </c>
       <c r="P8" s="8">
-        <v>4.8964733226890596E-3</v>
+        <v>3.6836307067628399E-3</v>
       </c>
       <c r="Q8" s="8">
-        <v>4.9517664405205998E-3</v>
+        <v>3.7382734277256399E-3</v>
       </c>
       <c r="R8" s="8">
-        <v>4.8654779778767301E-3</v>
+        <v>3.6405002404529302E-3</v>
       </c>
       <c r="S8" s="8">
-        <v>4.96790978681477E-3</v>
+        <v>3.70394096792992E-3</v>
       </c>
       <c r="T8" s="8">
-        <v>1.17868670194528E-4</v>
+        <v>7.0466721665522601E-5</v>
       </c>
       <c r="U8" s="8">
-        <v>-2.2691896974959399E-4</v>
+        <v>-1.65054953361904E-4</v>
       </c>
       <c r="V8" s="8">
-        <v>1.0507616215266E-4</v>
+        <v>-7.9536277947409296E-6</v>
       </c>
       <c r="W8" s="8">
-        <v>5.6208338789648999E-5</v>
+        <v>-6.18982082022266E-5</v>
       </c>
       <c r="X8" s="8">
-        <v>2.9904107335018302E-4</v>
+        <v>1.5629925725029999E-4</v>
       </c>
       <c r="Y8" s="8">
-        <v>-6.9781884904758496E-4</v>
+        <v>-5.4451905858729597E-4</v>
       </c>
       <c r="Z8" s="8">
-        <v>-3.7919712922618801E-5</v>
+        <v>-3.3986104429208902E-5</v>
       </c>
       <c r="AA8" s="8">
-        <v>1.5377625981489099E-5</v>
+        <v>7.1549796684478098E-6</v>
       </c>
       <c r="AB8" s="8">
-        <v>-1.3942838193155E-7</v>
+        <v>-6.9358125359632595E-8</v>
       </c>
       <c r="AC8" s="8">
-        <v>5.5429808852070404E-6</v>
+        <v>6.6583969087507302E-6</v>
       </c>
       <c r="AD8" s="8">
-        <v>-6.2674598652166803E-7</v>
+        <v>1.15372813028391E-6</v>
       </c>
       <c r="AE8" s="8">
-        <v>1.29370215620344E-4</v>
+        <v>9.4318092781603798E-5</v>
       </c>
       <c r="AF8" s="8">
-        <v>-3.9674796296594204E-3</v>
+        <v>-2.9119904647221199E-3</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
@@ -5556,97 +5557,97 @@
         <v>24</v>
       </c>
       <c r="B9" s="8">
-        <v>-7.1333019055259697E-2</v>
+        <v>-9.1136194334055204E-2</v>
       </c>
       <c r="C9" s="8">
-        <v>-1.16399598403884E-4</v>
+        <v>-5.6980063456238399E-5</v>
       </c>
       <c r="D9" s="8">
-        <v>-7.1231702273110396E-4</v>
+        <v>-4.4830984460138702E-4</v>
       </c>
       <c r="E9" s="8">
-        <v>3.7760747091908001E-4</v>
+        <v>2.0684718294199599E-4</v>
       </c>
       <c r="F9" s="8">
-        <v>-1.95094305549042E-4</v>
+        <v>-1.26285813992448E-4</v>
       </c>
       <c r="G9" s="8">
-        <v>-6.0221942485362903E-4</v>
+        <v>-4.5895451737053901E-4</v>
       </c>
       <c r="H9" s="8">
-        <v>-3.7353833085214302E-4</v>
+        <v>-3.70604266139672E-4</v>
       </c>
       <c r="I9" s="8">
-        <v>4.91706013151852E-3</v>
+        <v>3.6743190023038599E-3</v>
       </c>
       <c r="J9" s="8">
-        <v>7.7503179272565099E-3</v>
+        <v>5.8380388692748199E-3</v>
       </c>
       <c r="K9" s="8">
-        <v>4.8689232574635902E-3</v>
+        <v>3.6286156919623099E-3</v>
       </c>
       <c r="L9" s="8">
-        <v>4.9528222594198501E-3</v>
+        <v>3.6939218645868199E-3</v>
       </c>
       <c r="M9" s="8">
-        <v>4.9521212570981998E-3</v>
+        <v>3.6827497016285698E-3</v>
       </c>
       <c r="N9" s="8">
-        <v>4.79494238950954E-3</v>
+        <v>3.5904634475434302E-3</v>
       </c>
       <c r="O9" s="8">
-        <v>4.8196695716159798E-3</v>
+        <v>3.60305834835293E-3</v>
       </c>
       <c r="P9" s="8">
-        <v>4.88484648727322E-3</v>
+        <v>3.65240242553975E-3</v>
       </c>
       <c r="Q9" s="8">
-        <v>4.9464809206393803E-3</v>
+        <v>3.7008193299294099E-3</v>
       </c>
       <c r="R9" s="8">
-        <v>4.8760135961763897E-3</v>
+        <v>3.63079531134627E-3</v>
       </c>
       <c r="S9" s="8">
-        <v>4.9552445051715696E-3</v>
+        <v>3.6831324902577402E-3</v>
       </c>
       <c r="T9" s="8">
-        <v>3.4138618187333399E-4</v>
+        <v>2.9058430210802402E-4</v>
       </c>
       <c r="U9" s="8">
-        <v>2.7338272605515599E-5</v>
+        <v>-5.4928564757134402E-5</v>
       </c>
       <c r="V9" s="8">
-        <v>1.8501383716637001E-4</v>
+        <v>-2.8397989314200902E-6</v>
       </c>
       <c r="W9" s="8">
-        <v>1.2949505733784501E-4</v>
+        <v>-7.4528524240565999E-5</v>
       </c>
       <c r="X9" s="8">
-        <v>3.9706571421062602E-4</v>
+        <v>1.72442626212721E-4</v>
       </c>
       <c r="Y9" s="8">
-        <v>-7.1183901819658901E-4</v>
+        <v>-5.2613947803580301E-4</v>
       </c>
       <c r="Z9" s="8">
-        <v>-3.3634668775093298E-5</v>
+        <v>-2.9128536744634601E-5</v>
       </c>
       <c r="AA9" s="8">
-        <v>4.4795847847080399E-5</v>
+        <v>2.4342448627462001E-5</v>
       </c>
       <c r="AB9" s="8">
-        <v>-3.5386117864702402E-7</v>
+        <v>-1.83799025828355E-7</v>
       </c>
       <c r="AC9" s="8">
-        <v>-3.9788094929477201E-5</v>
+        <v>-2.1884028565649699E-5</v>
       </c>
       <c r="AD9" s="8">
-        <v>-2.47507421196567E-6</v>
+        <v>-9.6443425739680201E-7</v>
       </c>
       <c r="AE9" s="8">
-        <v>1.5554310311606301E-4</v>
+        <v>1.2351654348261799E-4</v>
       </c>
       <c r="AF9" s="8">
-        <v>-4.3283767875363704E-3</v>
+        <v>-3.0405545572973602E-3</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
@@ -5654,97 +5655,97 @@
         <v>25</v>
       </c>
       <c r="B10" s="8">
-        <v>-7.2435709640927798E-2</v>
+        <v>-2.7195450519272399E-2</v>
       </c>
       <c r="C10" s="8">
-        <v>-9.4741592403615603E-5</v>
+        <v>-3.3140607190495601E-5</v>
       </c>
       <c r="D10" s="8">
-        <v>-4.14376837020491E-4</v>
+        <v>-2.2976425546571001E-4</v>
       </c>
       <c r="E10" s="8">
-        <v>2.4763768093902E-4</v>
+        <v>2.3005346791499999E-4</v>
       </c>
       <c r="F10" s="8">
-        <v>-1.3353489737905601E-4</v>
+        <v>-5.5232721570482302E-5</v>
       </c>
       <c r="G10" s="8">
-        <v>-5.2754163679131398E-4</v>
+        <v>-3.8567926345713999E-4</v>
       </c>
       <c r="H10" s="8">
-        <v>-3.8067009212457397E-4</v>
+        <v>-3.33217203581994E-4</v>
       </c>
       <c r="I10" s="8">
-        <v>4.8906783378952802E-3</v>
+        <v>3.6653930960894999E-3</v>
       </c>
       <c r="J10" s="8">
-        <v>4.8689232574635902E-3</v>
+        <v>3.6286156919623099E-3</v>
       </c>
       <c r="K10" s="8">
-        <v>9.4965814870183792E-3</v>
+        <v>7.4416296907672801E-3</v>
       </c>
       <c r="L10" s="8">
-        <v>4.8692863814200201E-3</v>
+        <v>3.6377904707281801E-3</v>
       </c>
       <c r="M10" s="8">
-        <v>4.9250721041269301E-3</v>
+        <v>3.6716040119959799E-3</v>
       </c>
       <c r="N10" s="8">
-        <v>4.7747477954769302E-3</v>
+        <v>3.5812704645644799E-3</v>
       </c>
       <c r="O10" s="8">
-        <v>4.7688604152968904E-3</v>
+        <v>3.5780813461661599E-3</v>
       </c>
       <c r="P10" s="8">
-        <v>4.8522711076298001E-3</v>
+        <v>3.6326078509153399E-3</v>
       </c>
       <c r="Q10" s="8">
-        <v>4.9126725095242404E-3</v>
+        <v>3.6874740485083198E-3</v>
       </c>
       <c r="R10" s="8">
-        <v>4.8126308213113402E-3</v>
+        <v>3.5982278200898201E-3</v>
       </c>
       <c r="S10" s="8">
-        <v>4.9005215393465203E-3</v>
+        <v>3.6359723438137499E-3</v>
       </c>
       <c r="T10" s="8">
-        <v>3.5505137347886502E-4</v>
+        <v>2.55104704934409E-4</v>
       </c>
       <c r="U10" s="8">
-        <v>1.6498087515698601E-4</v>
+        <v>2.29935550132205E-5</v>
       </c>
       <c r="V10" s="8">
-        <v>3.6659091143644501E-4</v>
+        <v>1.22323228258313E-4</v>
       </c>
       <c r="W10" s="8">
-        <v>3.5743499612857601E-4</v>
+        <v>5.59177051410507E-5</v>
       </c>
       <c r="X10" s="8">
-        <v>5.8856010160817903E-4</v>
+        <v>3.1058008517539801E-4</v>
       </c>
       <c r="Y10" s="8">
-        <v>5.9577792176717097E-4</v>
+        <v>4.7062589410381498E-4</v>
       </c>
       <c r="Z10" s="8">
-        <v>-2.1321257993841702E-5</v>
+        <v>-2.38231760912954E-5</v>
       </c>
       <c r="AA10" s="8">
-        <v>1.0765165245551999E-5</v>
+        <v>8.7678985060418204E-6</v>
       </c>
       <c r="AB10" s="8">
-        <v>-3.3441185155948299E-8</v>
+        <v>-4.4605772097792299E-8</v>
       </c>
       <c r="AC10" s="8">
-        <v>4.7111321309611003E-6</v>
+        <v>4.6831607499127103E-6</v>
       </c>
       <c r="AD10" s="8">
-        <v>5.7162517755333003E-6</v>
+        <v>5.3646374898221998E-6</v>
       </c>
       <c r="AE10" s="8">
-        <v>1.04825224356768E-4</v>
+        <v>8.7184867609805801E-5</v>
       </c>
       <c r="AF10" s="8">
-        <v>-4.99602939742893E-3</v>
+        <v>-3.6637257779822902E-3</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
@@ -5752,97 +5753,97 @@
         <v>26</v>
       </c>
       <c r="B11" s="8">
-        <v>-8.0818617381666499E-2</v>
+        <v>-6.8579749080015504E-2</v>
       </c>
       <c r="C11" s="8">
-        <v>-5.4350626647645903E-5</v>
+        <v>-3.6026752548505101E-6</v>
       </c>
       <c r="D11" s="8">
-        <v>-5.5623871038439098E-4</v>
+        <v>-3.5132083779069502E-4</v>
       </c>
       <c r="E11" s="8">
-        <v>4.3657464900601198E-4</v>
+        <v>3.11404916713212E-4</v>
       </c>
       <c r="F11" s="8">
-        <v>-1.5390064258914599E-5</v>
+        <v>-1.07577635217511E-5</v>
       </c>
       <c r="G11" s="8">
-        <v>-6.8903916357526695E-4</v>
+        <v>-5.2028759380593999E-4</v>
       </c>
       <c r="H11" s="8">
-        <v>-4.8632167939121002E-4</v>
+        <v>-4.6890013442667E-4</v>
       </c>
       <c r="I11" s="8">
-        <v>4.9296372906032998E-3</v>
+        <v>3.6962821497148199E-3</v>
       </c>
       <c r="J11" s="8">
-        <v>4.9528222594198501E-3</v>
+        <v>3.6939218645868199E-3</v>
       </c>
       <c r="K11" s="8">
-        <v>4.8692863814200201E-3</v>
+        <v>3.6377904707281801E-3</v>
       </c>
       <c r="L11" s="8">
-        <v>8.2123164394421692E-3</v>
+        <v>6.2770916000853601E-3</v>
       </c>
       <c r="M11" s="8">
-        <v>4.9858636697659399E-3</v>
+        <v>3.71778270032705E-3</v>
       </c>
       <c r="N11" s="8">
-        <v>4.8209972387188802E-3</v>
+        <v>3.6232981218722099E-3</v>
       </c>
       <c r="O11" s="8">
-        <v>4.8183697414616502E-3</v>
+        <v>3.6179067364955999E-3</v>
       </c>
       <c r="P11" s="8">
-        <v>4.8789759550997196E-3</v>
+        <v>3.6606082614984801E-3</v>
       </c>
       <c r="Q11" s="8">
-        <v>4.98391431123565E-3</v>
+        <v>3.7404923805526599E-3</v>
       </c>
       <c r="R11" s="8">
-        <v>4.8758920271050801E-3</v>
+        <v>3.6428763452834301E-3</v>
       </c>
       <c r="S11" s="8">
-        <v>4.9459501357654702E-3</v>
+        <v>3.6828162446926999E-3</v>
       </c>
       <c r="T11" s="8">
-        <v>3.8451413468715799E-4</v>
+        <v>3.0105057974443901E-4</v>
       </c>
       <c r="U11" s="8">
-        <v>2.0280631048449199E-4</v>
+        <v>8.8777000104614905E-5</v>
       </c>
       <c r="V11" s="8">
-        <v>3.0899507230058799E-4</v>
+        <v>1.16377708589877E-4</v>
       </c>
       <c r="W11" s="8">
-        <v>3.7660345054941401E-4</v>
+        <v>1.03539477613254E-4</v>
       </c>
       <c r="X11" s="8">
-        <v>5.75733059709002E-4</v>
+        <v>3.1316394322403299E-4</v>
       </c>
       <c r="Y11" s="8">
-        <v>2.0118762423022301E-4</v>
+        <v>1.20153026031496E-4</v>
       </c>
       <c r="Z11" s="8">
-        <v>-4.7861067581385998E-5</v>
+        <v>-4.1123282692583602E-5</v>
       </c>
       <c r="AA11" s="8">
-        <v>4.6770773274575097E-5</v>
+        <v>3.0784171367229803E-5</v>
       </c>
       <c r="AB11" s="8">
-        <v>-3.5225352668302998E-7</v>
+        <v>-2.32806765575063E-7</v>
       </c>
       <c r="AC11" s="8">
-        <v>-2.2271571190318501E-5</v>
+        <v>-1.61945059632531E-5</v>
       </c>
       <c r="AD11" s="8">
-        <v>-1.78348677322715E-6</v>
+        <v>-9.71923573944943E-7</v>
       </c>
       <c r="AE11" s="8">
-        <v>1.1226244316264E-4</v>
+        <v>1.08484040202177E-4</v>
       </c>
       <c r="AF11" s="8">
-        <v>-4.7173784418936696E-3</v>
+        <v>-3.34205043482237E-3</v>
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
@@ -5850,97 +5851,97 @@
         <v>27</v>
       </c>
       <c r="B12" s="8">
-        <v>-2.66247102759536E-2</v>
+        <v>-7.9522681696701597E-2</v>
       </c>
       <c r="C12" s="8">
-        <v>-1.03792828150084E-5</v>
+        <v>-5.8135899523151103E-6</v>
       </c>
       <c r="D12" s="8">
-        <v>-6.7266191752578502E-4</v>
+        <v>-4.6152293938123498E-4</v>
       </c>
       <c r="E12" s="8">
-        <v>5.8783018712168101E-4</v>
+        <v>3.4570204999660303E-4</v>
       </c>
       <c r="F12" s="8">
-        <v>8.0183589488082006E-5</v>
+        <v>8.6543257663103203E-5</v>
       </c>
       <c r="G12" s="8">
-        <v>-7.8366353885107301E-4</v>
+        <v>-5.6973404853032604E-4</v>
       </c>
       <c r="H12" s="8">
-        <v>-6.8660318474704398E-4</v>
+        <v>-5.8122075101469902E-4</v>
       </c>
       <c r="I12" s="8">
-        <v>4.9603592623371599E-3</v>
+        <v>3.7101042049958901E-3</v>
       </c>
       <c r="J12" s="8">
-        <v>4.9521212570981998E-3</v>
+        <v>3.6827497016285698E-3</v>
       </c>
       <c r="K12" s="8">
-        <v>4.9250721041269301E-3</v>
+        <v>3.6716040119959799E-3</v>
       </c>
       <c r="L12" s="8">
-        <v>4.9858636697659399E-3</v>
+        <v>3.71778270032705E-3</v>
       </c>
       <c r="M12" s="8">
-        <v>9.1036519149018998E-3</v>
+        <v>6.8234212157236704E-3</v>
       </c>
       <c r="N12" s="8">
-        <v>4.83434460918816E-3</v>
+        <v>3.6178440583387698E-3</v>
       </c>
       <c r="O12" s="8">
-        <v>4.8394603686540598E-3</v>
+        <v>3.6136572669628799E-3</v>
       </c>
       <c r="P12" s="8">
-        <v>4.9132203769173101E-3</v>
+        <v>3.6832035897003401E-3</v>
       </c>
       <c r="Q12" s="8">
-        <v>4.9911997553037197E-3</v>
+        <v>3.74656928382823E-3</v>
       </c>
       <c r="R12" s="8">
-        <v>4.8856486455708496E-3</v>
+        <v>3.6373330072810299E-3</v>
       </c>
       <c r="S12" s="8">
-        <v>4.9740611510567098E-3</v>
+        <v>3.7049814789480301E-3</v>
       </c>
       <c r="T12" s="8">
-        <v>2.0297003995654899E-4</v>
+        <v>1.8924768415587301E-4</v>
       </c>
       <c r="U12" s="8">
-        <v>2.0847982173390699E-4</v>
+        <v>8.8665725766867197E-5</v>
       </c>
       <c r="V12" s="8">
-        <v>2.4800018501134501E-4</v>
+        <v>1.10730279763057E-4</v>
       </c>
       <c r="W12" s="8">
-        <v>4.20850471503258E-4</v>
+        <v>1.89091830047346E-4</v>
       </c>
       <c r="X12" s="8">
-        <v>4.9671034228580704E-4</v>
+        <v>3.18350819095063E-4</v>
       </c>
       <c r="Y12" s="8">
-        <v>-1.4670553689512399E-4</v>
+        <v>-6.7841435865638493E-5</v>
       </c>
       <c r="Z12" s="8">
-        <v>-2.70066441647624E-5</v>
+        <v>-2.7568287042084499E-5</v>
       </c>
       <c r="AA12" s="8">
-        <v>4.2996462274552398E-5</v>
+        <v>2.04241287357682E-5</v>
       </c>
       <c r="AB12" s="8">
-        <v>-3.2330155275160702E-7</v>
+        <v>-1.3118006608978299E-7</v>
       </c>
       <c r="AC12" s="8">
-        <v>-4.1565924680129503E-5</v>
+        <v>-2.7274544463754799E-5</v>
       </c>
       <c r="AD12" s="8">
-        <v>-2.6753411503209099E-6</v>
+        <v>-1.3377557896753101E-6</v>
       </c>
       <c r="AE12" s="8">
-        <v>2.10789727162438E-4</v>
+        <v>1.5480723694247199E-4</v>
       </c>
       <c r="AF12" s="8">
-        <v>-4.5881572585573698E-3</v>
+        <v>-3.0863304901270999E-3</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
@@ -5948,97 +5949,97 @@
         <v>28</v>
       </c>
       <c r="B13" s="8">
-        <v>-0.166602765271605</v>
+        <v>-0.17183044444259099</v>
       </c>
       <c r="C13" s="8">
-        <v>-2.63902686176086E-6</v>
+        <v>2.6292523201600701E-5</v>
       </c>
       <c r="D13" s="8">
-        <v>-5.2397664131760004E-4</v>
+        <v>-3.5275221770223402E-4</v>
       </c>
       <c r="E13" s="8">
-        <v>4.4859149736028699E-4</v>
+        <v>2.9448154059105697E-4</v>
       </c>
       <c r="F13" s="8">
-        <v>-4.6229899146876597E-5</v>
+        <v>2.2338614595099699E-5</v>
       </c>
       <c r="G13" s="8">
-        <v>-5.2772343135743102E-4</v>
+        <v>-4.2316898859286298E-4</v>
       </c>
       <c r="H13" s="8">
-        <v>-4.86744667460091E-4</v>
+        <v>-4.4318131596151499E-4</v>
       </c>
       <c r="I13" s="8">
-        <v>4.8257283805805398E-3</v>
+        <v>3.6277547096365201E-3</v>
       </c>
       <c r="J13" s="8">
-        <v>4.79494238950954E-3</v>
+        <v>3.5904634475434302E-3</v>
       </c>
       <c r="K13" s="8">
-        <v>4.7747477954769302E-3</v>
+        <v>3.5812704645644799E-3</v>
       </c>
       <c r="L13" s="8">
-        <v>4.8209972387188802E-3</v>
+        <v>3.6232981218722099E-3</v>
       </c>
       <c r="M13" s="8">
-        <v>4.83434460918816E-3</v>
+        <v>3.6178440583387698E-3</v>
       </c>
       <c r="N13" s="8">
-        <v>7.3173195766588197E-3</v>
+        <v>5.6839601067302003E-3</v>
       </c>
       <c r="O13" s="8">
-        <v>4.7023703525678898E-3</v>
+        <v>3.5366661971086102E-3</v>
       </c>
       <c r="P13" s="8">
-        <v>4.7660081423213903E-3</v>
+        <v>3.59051165682347E-3</v>
       </c>
       <c r="Q13" s="8">
-        <v>4.84705378381242E-3</v>
+        <v>3.6510796493132002E-3</v>
       </c>
       <c r="R13" s="8">
-        <v>4.7731495059121403E-3</v>
+        <v>3.5689831956946098E-3</v>
       </c>
       <c r="S13" s="8">
-        <v>4.79905604747411E-3</v>
+        <v>3.5864061330973798E-3</v>
       </c>
       <c r="T13" s="8">
-        <v>2.6033600430292001E-4</v>
+        <v>2.1059693020532199E-4</v>
       </c>
       <c r="U13" s="8">
-        <v>1.4253407316368899E-4</v>
+        <v>7.0933444677157204E-5</v>
       </c>
       <c r="V13" s="8">
-        <v>2.63078706415239E-4</v>
+        <v>1.15104077849468E-4</v>
       </c>
       <c r="W13" s="8">
-        <v>2.1263757006878301E-4</v>
+        <v>7.7272223311095799E-6</v>
       </c>
       <c r="X13" s="8">
-        <v>4.0674443862732398E-4</v>
+        <v>2.0951522786930599E-4</v>
       </c>
       <c r="Y13" s="8">
-        <v>-2.1564599842028901E-5</v>
+        <v>-2.03739851255387E-5</v>
       </c>
       <c r="Z13" s="8">
-        <v>-3.9139181867130601E-5</v>
+        <v>-3.5213531937796298E-5</v>
       </c>
       <c r="AA13" s="8">
-        <v>4.8440801622610499E-5</v>
+        <v>3.1758192246236301E-5</v>
       </c>
       <c r="AB13" s="8">
-        <v>-4.1475301244220901E-7</v>
+        <v>-2.7943379093036902E-7</v>
       </c>
       <c r="AC13" s="8">
-        <v>-3.80510178376622E-5</v>
+        <v>-2.5921318177962599E-5</v>
       </c>
       <c r="AD13" s="8">
-        <v>-3.6009848806514798E-6</v>
+        <v>-1.7770997084841599E-6</v>
       </c>
       <c r="AE13" s="8">
-        <v>1.7958724863632199E-4</v>
+        <v>1.6026663310050399E-4</v>
       </c>
       <c r="AF13" s="8">
-        <v>-4.4290039680673597E-3</v>
+        <v>-3.1617315106646999E-3</v>
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
@@ -6046,97 +6047,97 @@
         <v>29</v>
       </c>
       <c r="B14" s="8">
-        <v>-3.1215381840240801E-2</v>
+        <v>-5.6914780949895799E-2</v>
       </c>
       <c r="C14" s="8">
-        <v>-9.9363622412932599E-5</v>
+        <v>-3.1916735306552297E-5</v>
       </c>
       <c r="D14" s="8">
-        <v>-5.5506112148713397E-4</v>
+        <v>-3.5054121855327601E-4</v>
       </c>
       <c r="E14" s="8">
-        <v>4.0677706934950599E-4</v>
+        <v>2.6739695011598902E-4</v>
       </c>
       <c r="F14" s="8">
-        <v>-1.03273264004224E-4</v>
+        <v>-4.2191481593052299E-5</v>
       </c>
       <c r="G14" s="8">
-        <v>-5.4675858160080002E-4</v>
+        <v>-4.2519474578210702E-4</v>
       </c>
       <c r="H14" s="8">
-        <v>-3.8040131403236602E-4</v>
+        <v>-3.4991666551239397E-4</v>
       </c>
       <c r="I14" s="8">
-        <v>4.8206825441132802E-3</v>
+        <v>3.61994904942705E-3</v>
       </c>
       <c r="J14" s="8">
-        <v>4.8196695716159798E-3</v>
+        <v>3.60305834835293E-3</v>
       </c>
       <c r="K14" s="8">
-        <v>4.7688604152968904E-3</v>
+        <v>3.5780813461661599E-3</v>
       </c>
       <c r="L14" s="8">
-        <v>4.8183697414616502E-3</v>
+        <v>3.6179067364955999E-3</v>
       </c>
       <c r="M14" s="8">
-        <v>4.8394603686540598E-3</v>
+        <v>3.6136572669628799E-3</v>
       </c>
       <c r="N14" s="8">
-        <v>4.7023703525678898E-3</v>
+        <v>3.5366661971086102E-3</v>
       </c>
       <c r="O14" s="8">
-        <v>6.6424127929376603E-3</v>
+        <v>5.0174294117191504E-3</v>
       </c>
       <c r="P14" s="8">
-        <v>4.7928266171683798E-3</v>
+        <v>3.60481533575897E-3</v>
       </c>
       <c r="Q14" s="8">
-        <v>4.8637301008116803E-3</v>
+        <v>3.6613046382376799E-3</v>
       </c>
       <c r="R14" s="8">
-        <v>4.8124893733067402E-3</v>
+        <v>3.59903551776231E-3</v>
       </c>
       <c r="S14" s="8">
-        <v>4.7986633996432004E-3</v>
+        <v>3.5890105926193799E-3</v>
       </c>
       <c r="T14" s="8">
-        <v>2.4720089118391198E-4</v>
+        <v>2.12500321994609E-4</v>
       </c>
       <c r="U14" s="8">
-        <v>1.5300644969461099E-4</v>
+        <v>6.5047175705935901E-5</v>
       </c>
       <c r="V14" s="8">
-        <v>1.75726002946763E-4</v>
+        <v>2.8991814827594199E-5</v>
       </c>
       <c r="W14" s="8">
-        <v>1.44102312895738E-4</v>
+        <v>-3.4256943672093998E-5</v>
       </c>
       <c r="X14" s="8">
-        <v>3.2902404909209798E-4</v>
+        <v>1.44465411850755E-4</v>
       </c>
       <c r="Y14" s="8">
-        <v>-2.0198379228426999E-4</v>
+        <v>-1.2989506752020101E-4</v>
       </c>
       <c r="Z14" s="8">
-        <v>-4.2169182807177201E-5</v>
+        <v>-3.1161916154452298E-5</v>
       </c>
       <c r="AA14" s="8">
-        <v>4.0700433989505798E-5</v>
+        <v>3.0056493142876501E-5</v>
       </c>
       <c r="AB14" s="8">
-        <v>-3.5186698747759499E-7</v>
+        <v>-2.6997151693475101E-7</v>
       </c>
       <c r="AC14" s="8">
-        <v>-3.0025605176261102E-5</v>
+        <v>-1.9356988529694E-5</v>
       </c>
       <c r="AD14" s="8">
-        <v>-6.0834902577431698E-6</v>
+        <v>-3.3297926801775999E-6</v>
       </c>
       <c r="AE14" s="8">
-        <v>1.0183127722180401E-4</v>
+        <v>9.9770514449259805E-5</v>
       </c>
       <c r="AF14" s="8">
-        <v>-3.9710661631880704E-3</v>
+        <v>-3.04941863417782E-3</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
@@ -6144,97 +6145,97 @@
         <v>30</v>
       </c>
       <c r="B15" s="8">
-        <v>-2.4487393052353899E-2</v>
+        <v>-6.8317375500882294E-2</v>
       </c>
       <c r="C15" s="8">
-        <v>-5.9207400570414001E-5</v>
+        <v>-1.3920141205489E-5</v>
       </c>
       <c r="D15" s="8">
-        <v>-6.0942872218548499E-4</v>
+        <v>-3.9440505676415898E-4</v>
       </c>
       <c r="E15" s="8">
-        <v>4.5665169764451001E-4</v>
+        <v>3.22114963046491E-4</v>
       </c>
       <c r="F15" s="8">
-        <v>-9.8782636777001602E-5</v>
+        <v>-4.8724689555940298E-5</v>
       </c>
       <c r="G15" s="8">
-        <v>-5.5763362677569101E-4</v>
+        <v>-4.5651480665931599E-4</v>
       </c>
       <c r="H15" s="8">
-        <v>-3.1228086118793603E-4</v>
+        <v>-3.4582868039585799E-4</v>
       </c>
       <c r="I15" s="8">
-        <v>4.8964733226890596E-3</v>
+        <v>3.6836307067628399E-3</v>
       </c>
       <c r="J15" s="8">
-        <v>4.88484648727322E-3</v>
+        <v>3.65240242553975E-3</v>
       </c>
       <c r="K15" s="8">
-        <v>4.8522711076298001E-3</v>
+        <v>3.6326078509153399E-3</v>
       </c>
       <c r="L15" s="8">
-        <v>4.8789759550997196E-3</v>
+        <v>3.6606082614984801E-3</v>
       </c>
       <c r="M15" s="8">
-        <v>4.9132203769173101E-3</v>
+        <v>3.6832035897003401E-3</v>
       </c>
       <c r="N15" s="8">
-        <v>4.7660081423213903E-3</v>
+        <v>3.59051165682347E-3</v>
       </c>
       <c r="O15" s="8">
-        <v>4.7928266171683798E-3</v>
+        <v>3.60481533575897E-3</v>
       </c>
       <c r="P15" s="8">
-        <v>7.6527111657479097E-3</v>
+        <v>5.8966651948963696E-3</v>
       </c>
       <c r="Q15" s="8">
-        <v>4.9161193441138703E-3</v>
+        <v>3.7062791238492302E-3</v>
       </c>
       <c r="R15" s="8">
-        <v>4.8660822144284098E-3</v>
+        <v>3.6335672517614401E-3</v>
       </c>
       <c r="S15" s="8">
-        <v>4.8880652745892598E-3</v>
+        <v>3.6506563494569902E-3</v>
       </c>
       <c r="T15" s="8">
-        <v>4.6557522964846097E-4</v>
+        <v>3.2188948765598201E-4</v>
       </c>
       <c r="U15" s="8">
-        <v>1.58616439596469E-4</v>
+        <v>4.49211348629465E-5</v>
       </c>
       <c r="V15" s="8">
-        <v>2.61658617064542E-4</v>
+        <v>1.02602623044222E-4</v>
       </c>
       <c r="W15" s="8">
-        <v>2.8359671653344998E-4</v>
+        <v>4.3201772531197503E-5</v>
       </c>
       <c r="X15" s="8">
-        <v>5.3372440448698803E-4</v>
+        <v>2.72477586967644E-4</v>
       </c>
       <c r="Y15" s="8">
-        <v>-3.27370158724004E-4</v>
+        <v>-2.1155386442153201E-4</v>
       </c>
       <c r="Z15" s="8">
-        <v>-4.5730450361094003E-5</v>
+        <v>-3.8629289670829497E-5</v>
       </c>
       <c r="AA15" s="8">
-        <v>4.9743362690267503E-5</v>
+        <v>3.4304687460243302E-5</v>
       </c>
       <c r="AB15" s="8">
-        <v>-3.9877838251645799E-7</v>
+        <v>-2.8371600823174798E-7</v>
       </c>
       <c r="AC15" s="8">
-        <v>-2.1946171195734E-5</v>
+        <v>-1.32486692496256E-5</v>
       </c>
       <c r="AD15" s="8">
-        <v>-1.7093373471616401E-6</v>
+        <v>-8.7502828710036599E-7</v>
       </c>
       <c r="AE15" s="8">
-        <v>1.6744977284978299E-4</v>
+        <v>1.4781598336841001E-4</v>
       </c>
       <c r="AF15" s="8">
-        <v>-4.7488306469483897E-3</v>
+        <v>-3.41639667813341E-3</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
@@ -6242,97 +6243,97 @@
         <v>31</v>
       </c>
       <c r="B16" s="8">
-        <v>-4.0175955012486497E-2</v>
+        <v>2.7979239092005101E-2</v>
       </c>
       <c r="C16" s="8">
-        <v>1.8828056144282501E-5</v>
+        <v>7.0784726374946501E-6</v>
       </c>
       <c r="D16" s="8">
-        <v>-8.0115066736729905E-4</v>
+        <v>-6.1019892780987499E-4</v>
       </c>
       <c r="E16" s="8">
-        <v>7.7475942359961001E-4</v>
+        <v>6.5435228250584204E-4</v>
       </c>
       <c r="F16" s="8">
-        <v>1.9345962453120899E-4</v>
+        <v>1.5903834510351401E-4</v>
       </c>
       <c r="G16" s="8">
-        <v>-5.3898399279217696E-4</v>
+        <v>-3.9053190811033298E-4</v>
       </c>
       <c r="H16" s="8">
-        <v>-4.3244966480001702E-4</v>
+        <v>-4.19041373455933E-4</v>
       </c>
       <c r="I16" s="8">
-        <v>4.9517664405205998E-3</v>
+        <v>3.7382734277256399E-3</v>
       </c>
       <c r="J16" s="8">
-        <v>4.9464809206393803E-3</v>
+        <v>3.7008193299294099E-3</v>
       </c>
       <c r="K16" s="8">
-        <v>4.9126725095242404E-3</v>
+        <v>3.6874740485083198E-3</v>
       </c>
       <c r="L16" s="8">
-        <v>4.98391431123565E-3</v>
+        <v>3.7404923805526599E-3</v>
       </c>
       <c r="M16" s="8">
-        <v>4.9911997553037197E-3</v>
+        <v>3.74656928382823E-3</v>
       </c>
       <c r="N16" s="8">
-        <v>4.84705378381242E-3</v>
+        <v>3.6510796493132002E-3</v>
       </c>
       <c r="O16" s="8">
-        <v>4.8637301008116803E-3</v>
+        <v>3.6613046382376799E-3</v>
       </c>
       <c r="P16" s="8">
-        <v>4.9161193441138703E-3</v>
+        <v>3.7062791238492302E-3</v>
       </c>
       <c r="Q16" s="8">
-        <v>1.3264015199256201E-2</v>
+        <v>1.05928240895918E-2</v>
       </c>
       <c r="R16" s="8">
-        <v>4.8816361664901298E-3</v>
+        <v>3.6556594107903201E-3</v>
       </c>
       <c r="S16" s="8">
-        <v>4.9800728466450504E-3</v>
+        <v>3.7277507599967502E-3</v>
       </c>
       <c r="T16" s="8">
-        <v>2.7780627251527501E-4</v>
+        <v>1.7302794154127501E-4</v>
       </c>
       <c r="U16" s="8">
-        <v>-5.8901984543240802E-5</v>
+        <v>-1.3021485508586301E-4</v>
       </c>
       <c r="V16" s="8">
-        <v>7.3918964342981004E-5</v>
+        <v>-3.8916722242940501E-5</v>
       </c>
       <c r="W16" s="8">
-        <v>1.9222593505507899E-4</v>
+        <v>-3.6457373039728102E-5</v>
       </c>
       <c r="X16" s="8">
-        <v>4.5918504643472399E-4</v>
+        <v>2.2712555397529099E-4</v>
       </c>
       <c r="Y16" s="8">
-        <v>-4.43186962277778E-4</v>
+        <v>-3.6833839483740697E-4</v>
       </c>
       <c r="Z16" s="8">
-        <v>-1.6152441777825999E-5</v>
+        <v>-1.5899863080785099E-5</v>
       </c>
       <c r="AA16" s="8">
-        <v>6.6962399651288395E-5</v>
+        <v>5.3283980456599201E-5</v>
       </c>
       <c r="AB16" s="8">
-        <v>-5.3591319747416199E-7</v>
+        <v>-4.2294495287388402E-7</v>
       </c>
       <c r="AC16" s="8">
-        <v>-2.5704786345445799E-5</v>
+        <v>-1.5305125523319501E-5</v>
       </c>
       <c r="AD16" s="8">
-        <v>-3.4711754374417602E-7</v>
+        <v>8.4653209894722195E-7</v>
       </c>
       <c r="AE16" s="8">
-        <v>1.5264729666305299E-4</v>
+        <v>1.76127397211751E-4</v>
       </c>
       <c r="AF16" s="8">
-        <v>-5.6465546488757897E-3</v>
+        <v>-4.2994049611112502E-3</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
@@ -6340,97 +6341,97 @@
         <v>32</v>
       </c>
       <c r="B17" s="8">
-        <v>-5.8132721558237697E-2</v>
+        <v>-8.01329355410587E-2</v>
       </c>
       <c r="C17" s="8">
-        <v>-1.1829564444302599E-4</v>
+        <v>-5.1913341417064199E-5</v>
       </c>
       <c r="D17" s="8">
-        <v>-6.6449482002627297E-4</v>
+        <v>-4.2531167881112899E-4</v>
       </c>
       <c r="E17" s="8">
-        <v>3.6196407345823E-4</v>
+        <v>1.8643456883649201E-4</v>
       </c>
       <c r="F17" s="8">
-        <v>-2.7882665247920199E-4</v>
+        <v>-1.48122627785236E-4</v>
       </c>
       <c r="G17" s="8">
-        <v>-4.1045282850515598E-4</v>
+        <v>-3.40608746747858E-4</v>
       </c>
       <c r="H17" s="8">
-        <v>-1.5628089169628399E-4</v>
+        <v>-1.8354713762818101E-4</v>
       </c>
       <c r="I17" s="8">
-        <v>4.8654779778767301E-3</v>
+        <v>3.6405002404529302E-3</v>
       </c>
       <c r="J17" s="8">
-        <v>4.8760135961763897E-3</v>
+        <v>3.63079531134627E-3</v>
       </c>
       <c r="K17" s="8">
-        <v>4.8126308213113402E-3</v>
+        <v>3.5982278200898201E-3</v>
       </c>
       <c r="L17" s="8">
-        <v>4.8758920271050801E-3</v>
+        <v>3.6428763452834301E-3</v>
       </c>
       <c r="M17" s="8">
-        <v>4.8856486455708496E-3</v>
+        <v>3.6373330072810299E-3</v>
       </c>
       <c r="N17" s="8">
-        <v>4.7731495059121403E-3</v>
+        <v>3.5689831956946098E-3</v>
       </c>
       <c r="O17" s="8">
-        <v>4.8124893733067402E-3</v>
+        <v>3.59903551776231E-3</v>
       </c>
       <c r="P17" s="8">
-        <v>4.8660822144284098E-3</v>
+        <v>3.6335672517614401E-3</v>
       </c>
       <c r="Q17" s="8">
-        <v>4.8816361664901298E-3</v>
+        <v>3.6556594107903201E-3</v>
       </c>
       <c r="R17" s="8">
-        <v>1.0279037963647699E-2</v>
+        <v>7.5772220981151599E-3</v>
       </c>
       <c r="S17" s="8">
-        <v>4.8697484493990398E-3</v>
+        <v>3.6316966273550202E-3</v>
       </c>
       <c r="T17" s="8">
-        <v>1.8443809766261301E-4</v>
+        <v>1.7664596266606699E-4</v>
       </c>
       <c r="U17" s="8">
-        <v>-4.5639001536050598E-6</v>
+        <v>1.35419483380916E-5</v>
       </c>
       <c r="V17" s="8">
-        <v>3.9697280441727396E-6</v>
+        <v>-3.9023475577853197E-5</v>
       </c>
       <c r="W17" s="8">
-        <v>-1.9996438042124E-5</v>
+        <v>-9.1901591422994901E-5</v>
       </c>
       <c r="X17" s="8">
-        <v>3.22829203105524E-4</v>
+        <v>1.7418328243838901E-4</v>
       </c>
       <c r="Y17" s="8">
-        <v>-7.3890561767000096E-4</v>
+        <v>-3.5045715914234701E-4</v>
       </c>
       <c r="Z17" s="8">
-        <v>-2.11878228634332E-5</v>
+        <v>-1.3505716957335199E-5</v>
       </c>
       <c r="AA17" s="8">
-        <v>1.9688040213070699E-5</v>
+        <v>1.61817515153918E-5</v>
       </c>
       <c r="AB17" s="8">
-        <v>-1.6705108955779699E-7</v>
+        <v>-1.4383094386253899E-7</v>
       </c>
       <c r="AC17" s="8">
-        <v>1.3967176173467299E-5</v>
+        <v>7.5524382012530103E-6</v>
       </c>
       <c r="AD17" s="8">
-        <v>-3.74664897787857E-6</v>
+        <v>-2.0810114648482401E-6</v>
       </c>
       <c r="AE17" s="8">
-        <v>5.7211024127117701E-5</v>
+        <v>9.7167713338926502E-5</v>
       </c>
       <c r="AF17" s="8">
-        <v>-4.2919591708235599E-3</v>
+        <v>-3.30926235510124E-3</v>
       </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
@@ -6438,97 +6439,97 @@
         <v>33</v>
       </c>
       <c r="B18" s="8">
-        <v>-0.36185758061617401</v>
+        <v>-0.31910411702290298</v>
       </c>
       <c r="C18" s="8">
-        <v>-3.8159597474569099E-5</v>
+        <v>9.0654499959562297E-7</v>
       </c>
       <c r="D18" s="8">
-        <v>-8.4574341081580697E-4</v>
+        <v>-5.4483268097545504E-4</v>
       </c>
       <c r="E18" s="8">
-        <v>2.89766996693161E-4</v>
+        <v>1.5896051790660899E-4</v>
       </c>
       <c r="F18" s="8">
-        <v>-2.7584955475909499E-4</v>
+        <v>-1.61917970891495E-4</v>
       </c>
       <c r="G18" s="8">
-        <v>-5.0834864668053198E-4</v>
+        <v>-3.8424220541903001E-4</v>
       </c>
       <c r="H18" s="8">
-        <v>-7.3661028076579197E-4</v>
+        <v>-6.1258261392858502E-4</v>
       </c>
       <c r="I18" s="8">
-        <v>4.96790978681477E-3</v>
+        <v>3.70394096792992E-3</v>
       </c>
       <c r="J18" s="8">
-        <v>4.9552445051715696E-3</v>
+        <v>3.6831324902577402E-3</v>
       </c>
       <c r="K18" s="8">
-        <v>4.9005215393465203E-3</v>
+        <v>3.6359723438137499E-3</v>
       </c>
       <c r="L18" s="8">
-        <v>4.9459501357654702E-3</v>
+        <v>3.6828162446926999E-3</v>
       </c>
       <c r="M18" s="8">
-        <v>4.9740611510567098E-3</v>
+        <v>3.7049814789480301E-3</v>
       </c>
       <c r="N18" s="8">
-        <v>4.79905604747411E-3</v>
+        <v>3.5864061330973798E-3</v>
       </c>
       <c r="O18" s="8">
-        <v>4.7986633996432004E-3</v>
+        <v>3.5890105926193799E-3</v>
       </c>
       <c r="P18" s="8">
-        <v>4.8880652745892598E-3</v>
+        <v>3.6506563494569902E-3</v>
       </c>
       <c r="Q18" s="8">
-        <v>4.9800728466450504E-3</v>
+        <v>3.7277507599967502E-3</v>
       </c>
       <c r="R18" s="8">
-        <v>4.8697484493990398E-3</v>
+        <v>3.6316966273550202E-3</v>
       </c>
       <c r="S18" s="8">
-        <v>1.4553907874115099E-2</v>
+        <v>1.08103847681537E-2</v>
       </c>
       <c r="T18" s="8">
-        <v>2.0037343533792801E-4</v>
+        <v>1.9086654806898E-4</v>
       </c>
       <c r="U18" s="8">
-        <v>2.9497447954011799E-4</v>
+        <v>1.2727920474501299E-4</v>
       </c>
       <c r="V18" s="8">
-        <v>4.2981923942768201E-4</v>
+        <v>1.4480244629774599E-4</v>
       </c>
       <c r="W18" s="8">
-        <v>4.2787892501130998E-4</v>
+        <v>1.1134018192666599E-4</v>
       </c>
       <c r="X18" s="8">
-        <v>7.3016998890877705E-4</v>
+        <v>3.8494143341752499E-4</v>
       </c>
       <c r="Y18" s="8">
-        <v>-6.4175941832065903E-4</v>
+        <v>-5.1160190503336095E-4</v>
       </c>
       <c r="Z18" s="8">
-        <v>-1.58810188010869E-5</v>
+        <v>-1.8053239998575698E-5</v>
       </c>
       <c r="AA18" s="8">
-        <v>2.6776318544249002E-5</v>
+        <v>1.8281612615116899E-5</v>
       </c>
       <c r="AB18" s="8">
-        <v>-1.11104502723895E-7</v>
+        <v>-8.9271201703801602E-8</v>
       </c>
       <c r="AC18" s="8">
-        <v>-1.9960511563682401E-5</v>
+        <v>-1.5751065671979301E-5</v>
       </c>
       <c r="AD18" s="8">
-        <v>1.18052823990489E-5</v>
+        <v>6.3442488630703199E-6</v>
       </c>
       <c r="AE18" s="8">
-        <v>-5.8696423875529303E-5</v>
+        <v>2.7037100275640499E-6</v>
       </c>
       <c r="AF18" s="8">
-        <v>-5.3557541859268901E-3</v>
+        <v>-3.6254356706759902E-3</v>
       </c>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
@@ -6536,97 +6537,97 @@
         <v>16</v>
       </c>
       <c r="B19" s="8">
-        <v>5.3459589517501601E-3</v>
+        <v>-2.8136273810019902E-4</v>
       </c>
       <c r="C19" s="8">
-        <v>-2.1242328967870799E-4</v>
+        <v>-1.7042693690025399E-4</v>
       </c>
       <c r="D19" s="8">
-        <v>-2.44476234846575E-4</v>
+        <v>-1.5726936471822299E-4</v>
       </c>
       <c r="E19" s="8">
-        <v>-2.0946537737323801E-4</v>
+        <v>-2.12827260295729E-4</v>
       </c>
       <c r="F19" s="8">
-        <v>-3.9731775296312199E-5</v>
+        <v>-2.7993404341663698E-5</v>
       </c>
       <c r="G19" s="8">
-        <v>-2.2342855962618501E-4</v>
+        <v>-1.90048164124522E-4</v>
       </c>
       <c r="H19" s="8">
-        <v>-1.3655058035892299E-4</v>
+        <v>-1.2664173552619299E-4</v>
       </c>
       <c r="I19" s="8">
-        <v>1.17868670194528E-4</v>
+        <v>7.0466721665522601E-5</v>
       </c>
       <c r="J19" s="8">
-        <v>3.4138618187333399E-4</v>
+        <v>2.9058430210802402E-4</v>
       </c>
       <c r="K19" s="8">
-        <v>3.5505137347886502E-4</v>
+        <v>2.55104704934409E-4</v>
       </c>
       <c r="L19" s="8">
-        <v>3.8451413468715799E-4</v>
+        <v>3.0105057974443901E-4</v>
       </c>
       <c r="M19" s="8">
-        <v>2.0297003995654899E-4</v>
+        <v>1.8924768415587301E-4</v>
       </c>
       <c r="N19" s="8">
-        <v>2.6033600430292001E-4</v>
+        <v>2.1059693020532199E-4</v>
       </c>
       <c r="O19" s="8">
-        <v>2.4720089118391198E-4</v>
+        <v>2.12500321994609E-4</v>
       </c>
       <c r="P19" s="8">
-        <v>4.6557522964846097E-4</v>
+        <v>3.2188948765598201E-4</v>
       </c>
       <c r="Q19" s="8">
-        <v>2.7780627251527501E-4</v>
+        <v>1.7302794154127501E-4</v>
       </c>
       <c r="R19" s="8">
-        <v>1.8443809766261301E-4</v>
+        <v>1.7664596266606699E-4</v>
       </c>
       <c r="S19" s="8">
-        <v>2.0037343533792801E-4</v>
+        <v>1.9086654806898E-4</v>
       </c>
       <c r="T19" s="8">
-        <v>3.25524949887204E-3</v>
+        <v>2.1563162627564101E-3</v>
       </c>
       <c r="U19" s="8">
-        <v>2.61658055811279E-4</v>
+        <v>1.5044795638907699E-4</v>
       </c>
       <c r="V19" s="8">
-        <v>2.7950972388213099E-4</v>
+        <v>1.69685104190843E-4</v>
       </c>
       <c r="W19" s="8">
-        <v>3.4391708714884999E-4</v>
+        <v>2.2195458470309601E-4</v>
       </c>
       <c r="X19" s="8">
-        <v>4.0388851438170903E-4</v>
+        <v>2.41879342314524E-4</v>
       </c>
       <c r="Y19" s="8">
-        <v>-1.5548564854924001E-5</v>
+        <v>-5.6890612907485797E-5</v>
       </c>
       <c r="Z19" s="8">
-        <v>-2.0674534998908601E-5</v>
+        <v>-2.1045161391780598E-5</v>
       </c>
       <c r="AA19" s="8">
-        <v>3.8778006033768097E-5</v>
+        <v>4.3348141485591701E-5</v>
       </c>
       <c r="AB19" s="8">
-        <v>-2.1422466781597199E-7</v>
+        <v>-2.94314048158248E-7</v>
       </c>
       <c r="AC19" s="8">
-        <v>-3.18285968860809E-5</v>
+        <v>-1.9989521205405801E-5</v>
       </c>
       <c r="AD19" s="8">
-        <v>-6.4599382033204897E-6</v>
+        <v>-4.9519808537223396E-6</v>
       </c>
       <c r="AE19" s="8">
-        <v>-8.0821919107185804E-6</v>
+        <v>2.9485886840635E-6</v>
       </c>
       <c r="AF19" s="8">
-        <v>-7.4725403196196198E-4</v>
+        <v>-8.2595513948921604E-4</v>
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
@@ -6634,97 +6635,97 @@
         <v>36</v>
       </c>
       <c r="B20" s="8">
-        <v>1.19241542950945E-2</v>
+        <v>-1.3540905833991699E-2</v>
       </c>
       <c r="C20" s="8">
-        <v>-1.28929979797121E-4</v>
+        <v>-1.06933575513096E-4</v>
       </c>
       <c r="D20" s="8">
-        <v>2.5523831405678999E-5</v>
+        <v>-1.7628097143113999E-5</v>
       </c>
       <c r="E20" s="8">
-        <v>1.9055926048402099E-4</v>
+        <v>1.3180405573850801E-4</v>
       </c>
       <c r="F20" s="8">
-        <v>5.81332560639315E-5</v>
+        <v>3.1765119593700298E-5</v>
       </c>
       <c r="G20" s="8">
-        <v>-1.04632177757973E-4</v>
+        <v>-8.0763238596518396E-5</v>
       </c>
       <c r="H20" s="8">
-        <v>-3.9061091234269703E-5</v>
+        <v>-1.3357685690987399E-5</v>
       </c>
       <c r="I20" s="8">
-        <v>-2.2691896974959399E-4</v>
+        <v>-1.65054953361904E-4</v>
       </c>
       <c r="J20" s="8">
-        <v>2.7338272605515599E-5</v>
+        <v>-5.4928564757134402E-5</v>
       </c>
       <c r="K20" s="8">
-        <v>1.6498087515698601E-4</v>
+        <v>2.29935550132205E-5</v>
       </c>
       <c r="L20" s="8">
-        <v>2.0280631048449199E-4</v>
+        <v>8.8777000104614905E-5</v>
       </c>
       <c r="M20" s="8">
-        <v>2.0847982173390699E-4</v>
+        <v>8.8665725766867197E-5</v>
       </c>
       <c r="N20" s="8">
-        <v>1.4253407316368899E-4</v>
+        <v>7.0933444677157204E-5</v>
       </c>
       <c r="O20" s="8">
-        <v>1.5300644969461099E-4</v>
+        <v>6.5047175705935901E-5</v>
       </c>
       <c r="P20" s="8">
-        <v>1.58616439596469E-4</v>
+        <v>4.49211348629465E-5</v>
       </c>
       <c r="Q20" s="8">
-        <v>-5.8901984543240802E-5</v>
+        <v>-1.3021485508586301E-4</v>
       </c>
       <c r="R20" s="8">
-        <v>-4.5639001536050598E-6</v>
+        <v>1.35419483380916E-5</v>
       </c>
       <c r="S20" s="8">
-        <v>2.9497447954011799E-4</v>
+        <v>1.2727920474501299E-4</v>
       </c>
       <c r="T20" s="8">
-        <v>2.61658055811279E-4</v>
+        <v>1.5044795638907699E-4</v>
       </c>
       <c r="U20" s="8">
-        <v>3.7294848193129598E-3</v>
+        <v>2.7414331718500899E-3</v>
       </c>
       <c r="V20" s="8">
-        <v>2.40164122437889E-3</v>
+        <v>1.75532650285816E-3</v>
       </c>
       <c r="W20" s="8">
-        <v>2.3965140779372402E-3</v>
+        <v>1.7425556298784201E-3</v>
       </c>
       <c r="X20" s="8">
-        <v>2.3494558132191E-3</v>
+        <v>1.7038493251756799E-3</v>
       </c>
       <c r="Y20" s="8">
-        <v>4.4541354921536099E-4</v>
+        <v>3.5177310421854801E-4</v>
       </c>
       <c r="Z20" s="8">
-        <v>-1.61364046784057E-5</v>
+        <v>-1.5544439150787701E-5</v>
       </c>
       <c r="AA20" s="8">
-        <v>5.8067607343704796E-6</v>
+        <v>-7.7485180559398298E-7</v>
       </c>
       <c r="AB20" s="8">
-        <v>1.6785398136138201E-8</v>
+        <v>5.8901365886500302E-8</v>
       </c>
       <c r="AC20" s="8">
-        <v>-9.8318830310963701E-6</v>
+        <v>-6.2973314165602897E-6</v>
       </c>
       <c r="AD20" s="8">
-        <v>-3.29264052820027E-6</v>
+        <v>-1.1643442175534399E-6</v>
       </c>
       <c r="AE20" s="8">
-        <v>1.1429896866467399E-6</v>
+        <v>-3.09401121375623E-6</v>
       </c>
       <c r="AF20" s="8">
-        <v>-2.2103235855487598E-3</v>
+        <v>-1.41664342203662E-3</v>
       </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">
@@ -6732,97 +6733,97 @@
         <v>37</v>
       </c>
       <c r="B21" s="8">
-        <v>-2.74555413885622E-2</v>
+        <v>-5.8437331079687703E-2</v>
       </c>
       <c r="C21" s="8">
-        <v>1.1912362644709499E-5</v>
+        <v>1.91159661513898E-6</v>
       </c>
       <c r="D21" s="8">
-        <v>-2.6638431963693399E-4</v>
+        <v>-2.35190709147246E-4</v>
       </c>
       <c r="E21" s="8">
-        <v>3.2630455617718398E-4</v>
+        <v>2.8501890220112902E-4</v>
       </c>
       <c r="F21" s="8">
-        <v>1.7026975078599099E-4</v>
+        <v>1.1021180503455699E-4</v>
       </c>
       <c r="G21" s="8">
-        <v>-4.2819949118650899E-5</v>
+        <v>-3.1488974456466399E-5</v>
       </c>
       <c r="H21" s="8">
-        <v>1.36876311242743E-4</v>
+        <v>1.4670503203129001E-4</v>
       </c>
       <c r="I21" s="8">
-        <v>1.0507616215266E-4</v>
+        <v>-7.9536277947409296E-6</v>
       </c>
       <c r="J21" s="8">
-        <v>1.8501383716637001E-4</v>
+        <v>-2.8397989314200902E-6</v>
       </c>
       <c r="K21" s="8">
-        <v>3.6659091143644501E-4</v>
+        <v>1.22323228258313E-4</v>
       </c>
       <c r="L21" s="8">
-        <v>3.0899507230058799E-4</v>
+        <v>1.16377708589877E-4</v>
       </c>
       <c r="M21" s="8">
-        <v>2.4800018501134501E-4</v>
+        <v>1.10730279763057E-4</v>
       </c>
       <c r="N21" s="8">
-        <v>2.63078706415239E-4</v>
+        <v>1.15104077849468E-4</v>
       </c>
       <c r="O21" s="8">
-        <v>1.75726002946763E-4</v>
+        <v>2.8991814827594199E-5</v>
       </c>
       <c r="P21" s="8">
-        <v>2.61658617064542E-4</v>
+        <v>1.02602623044222E-4</v>
       </c>
       <c r="Q21" s="8">
-        <v>7.3918964342981004E-5</v>
+        <v>-3.8916722242940501E-5</v>
       </c>
       <c r="R21" s="8">
-        <v>3.9697280441727396E-6</v>
+        <v>-3.9023475577853197E-5</v>
       </c>
       <c r="S21" s="8">
-        <v>4.2981923942768201E-4</v>
+        <v>1.4480244629774599E-4</v>
       </c>
       <c r="T21" s="8">
-        <v>2.7950972388213099E-4</v>
+        <v>1.69685104190843E-4</v>
       </c>
       <c r="U21" s="8">
-        <v>2.40164122437889E-3</v>
+        <v>1.75532650285816E-3</v>
       </c>
       <c r="V21" s="8">
-        <v>3.8670270820361499E-3</v>
+        <v>2.8750316698433901E-3</v>
       </c>
       <c r="W21" s="8">
-        <v>2.7108047775130499E-3</v>
+        <v>2.0107691173380099E-3</v>
       </c>
       <c r="X21" s="8">
-        <v>2.6697091518887999E-3</v>
+        <v>1.9630808947426201E-3</v>
       </c>
       <c r="Y21" s="8">
-        <v>6.3008111484256796E-4</v>
+        <v>4.62752440749351E-4</v>
       </c>
       <c r="Z21" s="8">
-        <v>-1.08559109154975E-5</v>
+        <v>-4.3231121222062101E-6</v>
       </c>
       <c r="AA21" s="8">
-        <v>7.6812333750776906E-6</v>
+        <v>3.55431784952156E-6</v>
       </c>
       <c r="AB21" s="8">
-        <v>8.5731017040313501E-9</v>
+        <v>2.5441536155777301E-8</v>
       </c>
       <c r="AC21" s="8">
-        <v>-1.62687339521438E-6</v>
+        <v>-1.89745777961124E-6</v>
       </c>
       <c r="AD21" s="8">
-        <v>-1.01962893170838E-6</v>
+        <v>3.5107206495501398E-7</v>
       </c>
       <c r="AE21" s="8">
-        <v>6.3597273331523601E-5</v>
+        <v>5.2607278529689499E-5</v>
       </c>
       <c r="AF21" s="8">
-        <v>-2.8409735738362499E-3</v>
+        <v>-2.023016610261E-3</v>
       </c>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.25">
@@ -6830,97 +6831,97 @@
         <v>39</v>
       </c>
       <c r="B22" s="8">
-        <v>-5.7946877117288402E-2</v>
+        <v>-9.2359153912809702E-2</v>
       </c>
       <c r="C22" s="8">
-        <v>1.6869150462134699E-4</v>
+        <v>1.17173090250836E-4</v>
       </c>
       <c r="D22" s="8">
-        <v>-4.60062817506805E-4</v>
+        <v>-3.9707618216626098E-4</v>
       </c>
       <c r="E22" s="8">
-        <v>4.2819227027188499E-4</v>
+        <v>3.6482712876218898E-4</v>
       </c>
       <c r="F22" s="8">
-        <v>2.1032483690185401E-4</v>
+        <v>1.75757031507802E-4</v>
       </c>
       <c r="G22" s="8">
-        <v>1.26938335667565E-5</v>
+        <v>2.8661231781060401E-5</v>
       </c>
       <c r="H22" s="8">
-        <v>2.8534020577091802E-4</v>
+        <v>3.0335887083627803E-4</v>
       </c>
       <c r="I22" s="8">
-        <v>5.6208338789648999E-5</v>
+        <v>-6.18982082022266E-5</v>
       </c>
       <c r="J22" s="8">
-        <v>1.2949505733784501E-4</v>
+        <v>-7.4528524240565999E-5</v>
       </c>
       <c r="K22" s="8">
-        <v>3.5743499612857601E-4</v>
+        <v>5.59177051410507E-5</v>
       </c>
       <c r="L22" s="8">
-        <v>3.7660345054941401E-4</v>
+        <v>1.03539477613254E-4</v>
       </c>
       <c r="M22" s="8">
-        <v>4.20850471503258E-4</v>
+        <v>1.89091830047346E-4</v>
       </c>
       <c r="N22" s="8">
-        <v>2.1263757006878301E-4</v>
+        <v>7.7272223311095799E-6</v>
       </c>
       <c r="O22" s="8">
-        <v>1.44102312895738E-4</v>
+        <v>-3.4256943672093998E-5</v>
       </c>
       <c r="P22" s="8">
-        <v>2.8359671653344998E-4</v>
+        <v>4.3201772531197503E-5</v>
       </c>
       <c r="Q22" s="8">
-        <v>1.9222593505507899E-4</v>
+        <v>-3.6457373039728102E-5</v>
       </c>
       <c r="R22" s="8">
-        <v>-1.9996438042124E-5</v>
+        <v>-9.1901591422994901E-5</v>
       </c>
       <c r="S22" s="8">
-        <v>4.2787892501130998E-4</v>
+        <v>1.1134018192666599E-4</v>
       </c>
       <c r="T22" s="8">
-        <v>3.4391708714884999E-4</v>
+        <v>2.2195458470309601E-4</v>
       </c>
       <c r="U22" s="8">
-        <v>2.3965140779372402E-3</v>
+        <v>1.7425556298784201E-3</v>
       </c>
       <c r="V22" s="8">
-        <v>2.7108047775130499E-3</v>
+        <v>2.0107691173380099E-3</v>
       </c>
       <c r="W22" s="8">
-        <v>4.0940693610557501E-3</v>
+        <v>3.0973622262788301E-3</v>
       </c>
       <c r="X22" s="8">
-        <v>2.8896405569067102E-3</v>
+        <v>2.1647754761515599E-3</v>
       </c>
       <c r="Y22" s="8">
-        <v>7.5801820482515896E-4</v>
+        <v>4.4949877068388601E-4</v>
       </c>
       <c r="Z22" s="8">
-        <v>1.08416010636646E-5</v>
+        <v>8.1752607270381502E-6</v>
       </c>
       <c r="AA22" s="8">
-        <v>4.9036715918067804E-6</v>
+        <v>-9.9580742348248902E-7</v>
       </c>
       <c r="AB22" s="8">
-        <v>4.1038573731187402E-8</v>
+        <v>7.8676433748307596E-8</v>
       </c>
       <c r="AC22" s="8">
-        <v>-3.60192170009771E-6</v>
+        <v>-1.4038264992738799E-7</v>
       </c>
       <c r="AD22" s="8">
-        <v>-3.82554767037291E-6</v>
+        <v>-1.5246218719420099E-6</v>
       </c>
       <c r="AE22" s="8">
-        <v>2.79940389253745E-5</v>
+        <v>-2.30135253225843E-6</v>
       </c>
       <c r="AF22" s="8">
-        <v>-3.08464000034487E-3</v>
+        <v>-2.1170347658758001E-3</v>
       </c>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.25">
@@ -6928,97 +6929,97 @@
         <v>40</v>
       </c>
       <c r="B23" s="8">
-        <v>-0.10765163368658601</v>
+        <v>-0.11490847119806299</v>
       </c>
       <c r="C23" s="8">
-        <v>3.5420281375932698E-4</v>
+        <v>2.5661305439669699E-4</v>
       </c>
       <c r="D23" s="8">
-        <v>-5.7627961049298404E-4</v>
+        <v>-4.6418451004554001E-4</v>
       </c>
       <c r="E23" s="8">
-        <v>4.2022039204532298E-4</v>
+        <v>3.4535045012430802E-4</v>
       </c>
       <c r="F23" s="8">
-        <v>2.7891371757865702E-4</v>
+        <v>2.32170272959106E-4</v>
       </c>
       <c r="G23" s="8">
-        <v>2.9569886621756702E-4</v>
+        <v>2.5053514890331402E-4</v>
       </c>
       <c r="H23" s="8">
-        <v>6.5824210999291003E-4</v>
+        <v>5.6827631859252003E-4</v>
       </c>
       <c r="I23" s="8">
-        <v>2.9904107335018302E-4</v>
+        <v>1.5629925725029999E-4</v>
       </c>
       <c r="J23" s="8">
-        <v>3.9706571421062602E-4</v>
+        <v>1.72442626212721E-4</v>
       </c>
       <c r="K23" s="8">
-        <v>5.8856010160817903E-4</v>
+        <v>3.1058008517539801E-4</v>
       </c>
       <c r="L23" s="8">
-        <v>5.75733059709002E-4</v>
+        <v>3.1316394322403299E-4</v>
       </c>
       <c r="M23" s="8">
-        <v>4.9671034228580704E-4</v>
+        <v>3.18350819095063E-4</v>
       </c>
       <c r="N23" s="8">
-        <v>4.0674443862732398E-4</v>
+        <v>2.0951522786930599E-4</v>
       </c>
       <c r="O23" s="8">
-        <v>3.2902404909209798E-4</v>
+        <v>1.44465411850755E-4</v>
       </c>
       <c r="P23" s="8">
-        <v>5.3372440448698803E-4</v>
+        <v>2.72477586967644E-4</v>
       </c>
       <c r="Q23" s="8">
-        <v>4.5918504643472399E-4</v>
+        <v>2.2712555397529099E-4</v>
       </c>
       <c r="R23" s="8">
-        <v>3.22829203105524E-4</v>
+        <v>1.7418328243838901E-4</v>
       </c>
       <c r="S23" s="8">
-        <v>7.3016998890877705E-4</v>
+        <v>3.8494143341752499E-4</v>
       </c>
       <c r="T23" s="8">
-        <v>4.0388851438170903E-4</v>
+        <v>2.41879342314524E-4</v>
       </c>
       <c r="U23" s="8">
-        <v>2.3494558132191E-3</v>
+        <v>1.7038493251756799E-3</v>
       </c>
       <c r="V23" s="8">
-        <v>2.6697091518887999E-3</v>
+        <v>1.9630808947426201E-3</v>
       </c>
       <c r="W23" s="8">
-        <v>2.8896405569067102E-3</v>
+        <v>2.1647754761515599E-3</v>
       </c>
       <c r="X23" s="8">
-        <v>4.1143828068329596E-3</v>
+        <v>3.0884208762260701E-3</v>
       </c>
       <c r="Y23" s="8">
-        <v>4.8931290330653005E-4</v>
+        <v>3.3943898569653602E-4</v>
       </c>
       <c r="Z23" s="8">
-        <v>1.4938019577859699E-6</v>
+        <v>2.7763091305072701E-6</v>
       </c>
       <c r="AA23" s="8">
-        <v>1.15262719514252E-5</v>
+        <v>3.7883514038165999E-6</v>
       </c>
       <c r="AB23" s="8">
-        <v>-6.6715033595401904E-8</v>
+        <v>-1.3253464341926199E-9</v>
       </c>
       <c r="AC23" s="8">
-        <v>3.3672766714307099E-7</v>
+        <v>-7.9601118039708399E-9</v>
       </c>
       <c r="AD23" s="8">
-        <v>-7.67978569468998E-6</v>
+        <v>-4.1293388728434297E-6</v>
       </c>
       <c r="AE23" s="8">
-        <v>-1.69638255491436E-5</v>
+        <v>-2.4996167309672399E-5</v>
       </c>
       <c r="AF23" s="8">
-        <v>-3.3052825074266099E-3</v>
+        <v>-2.3505563205864898E-3</v>
       </c>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.25">
@@ -7026,97 +7027,97 @@
         <v>47</v>
       </c>
       <c r="B24" s="8">
-        <v>1.6940540716511301</v>
+        <v>1.67744740400946</v>
       </c>
       <c r="C24" s="8">
-        <v>-3.2704333110136102E-4</v>
+        <v>-2.2776585886313499E-4</v>
       </c>
       <c r="D24" s="8">
-        <v>8.5721246069600998E-4</v>
+        <v>6.2970740391318899E-4</v>
       </c>
       <c r="E24" s="8">
-        <v>-1.89962332863713E-4</v>
+        <v>-2.0417905428785099E-4</v>
       </c>
       <c r="F24" s="8">
-        <v>-6.20921941204557E-5</v>
+        <v>-1.03556653835802E-4</v>
       </c>
       <c r="G24" s="8">
-        <v>-1.9854278345841201E-4</v>
+        <v>-1.3187972664026299E-4</v>
       </c>
       <c r="H24" s="8">
-        <v>-1.26608064496211E-4</v>
+        <v>-9.2684217219427404E-5</v>
       </c>
       <c r="I24" s="8">
-        <v>-6.9781884904758496E-4</v>
+        <v>-5.4451905858729597E-4</v>
       </c>
       <c r="J24" s="8">
-        <v>-7.1183901819658901E-4</v>
+        <v>-5.2613947803580301E-4</v>
       </c>
       <c r="K24" s="8">
-        <v>5.9577792176717097E-4</v>
+        <v>4.7062589410381498E-4</v>
       </c>
       <c r="L24" s="8">
-        <v>2.0118762423022301E-4</v>
+        <v>1.20153026031496E-4</v>
       </c>
       <c r="M24" s="8">
-        <v>-1.4670553689512399E-4</v>
+        <v>-6.7841435865638493E-5</v>
       </c>
       <c r="N24" s="8">
-        <v>-2.1564599842028901E-5</v>
+        <v>-2.03739851255387E-5</v>
       </c>
       <c r="O24" s="8">
-        <v>-2.0198379228426999E-4</v>
+        <v>-1.2989506752020101E-4</v>
       </c>
       <c r="P24" s="8">
-        <v>-3.27370158724004E-4</v>
+        <v>-2.1155386442153201E-4</v>
       </c>
       <c r="Q24" s="8">
-        <v>-4.43186962277778E-4</v>
+        <v>-3.6833839483740697E-4</v>
       </c>
       <c r="R24" s="8">
-        <v>-7.3890561767000096E-4</v>
+        <v>-3.5045715914234701E-4</v>
       </c>
       <c r="S24" s="8">
-        <v>-6.4175941832065903E-4</v>
+        <v>-5.1160190503336095E-4</v>
       </c>
       <c r="T24" s="8">
-        <v>-1.5548564854924001E-5</v>
+        <v>-5.6890612907485797E-5</v>
       </c>
       <c r="U24" s="8">
-        <v>4.4541354921536099E-4</v>
+        <v>3.5177310421854801E-4</v>
       </c>
       <c r="V24" s="8">
-        <v>6.3008111484256796E-4</v>
+        <v>4.62752440749351E-4</v>
       </c>
       <c r="W24" s="8">
-        <v>7.5801820482515896E-4</v>
+        <v>4.4949877068388601E-4</v>
       </c>
       <c r="X24" s="8">
-        <v>4.8931290330653005E-4</v>
+        <v>3.3943898569653602E-4</v>
       </c>
       <c r="Y24" s="8">
-        <v>2.8639018499865901E-2</v>
+        <v>2.1353217180365199E-2</v>
       </c>
       <c r="Z24" s="8">
-        <v>3.0427461575922E-5</v>
+        <v>1.0191418051885299E-5</v>
       </c>
       <c r="AA24" s="8">
-        <v>-1.13531822386823E-4</v>
+        <v>-9.3111197209676402E-5</v>
       </c>
       <c r="AB24" s="8">
-        <v>1.2905898832123601E-6</v>
+        <v>1.0366058796827001E-6</v>
       </c>
       <c r="AC24" s="8">
-        <v>-8.7595251560827796E-5</v>
+        <v>-6.7511039266497305E-5</v>
       </c>
       <c r="AD24" s="8">
-        <v>8.5997175046871295E-5</v>
+        <v>6.6298046674749102E-5</v>
       </c>
       <c r="AE24" s="8">
-        <v>-6.1995988585808299E-5</v>
+        <v>-5.02039356084404E-5</v>
       </c>
       <c r="AF24" s="8">
-        <v>-2.86707906624437E-3</v>
+        <v>-1.7936134470325799E-3</v>
       </c>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.25">
@@ -7124,97 +7125,97 @@
         <v>38</v>
       </c>
       <c r="B25" s="8">
-        <v>4.3528188179301701E-2</v>
+        <v>2.8439779796908499E-2</v>
       </c>
       <c r="C25" s="8">
-        <v>2.5770534110842701E-5</v>
+        <v>1.7418917226673301E-5</v>
       </c>
       <c r="D25" s="8">
-        <v>-2.4265473526926501E-5</v>
+        <v>-2.1762751755166099E-5</v>
       </c>
       <c r="E25" s="8">
-        <v>-9.91938982984867E-6</v>
+        <v>1.7149527807957399E-6</v>
       </c>
       <c r="F25" s="8">
-        <v>7.8306114194152597E-6</v>
+        <v>3.1585411834741901E-6</v>
       </c>
       <c r="G25" s="8">
-        <v>2.4286068127837401E-5</v>
+        <v>2.04754450575988E-5</v>
       </c>
       <c r="H25" s="8">
-        <v>5.4445328476127101E-5</v>
+        <v>4.91463903769168E-5</v>
       </c>
       <c r="I25" s="8">
-        <v>-3.7919712922618801E-5</v>
+        <v>-3.3986104429208902E-5</v>
       </c>
       <c r="J25" s="8">
-        <v>-3.3634668775093298E-5</v>
+        <v>-2.9128536744634601E-5</v>
       </c>
       <c r="K25" s="8">
-        <v>-2.1321257993841702E-5</v>
+        <v>-2.38231760912954E-5</v>
       </c>
       <c r="L25" s="8">
-        <v>-4.7861067581385998E-5</v>
+        <v>-4.1123282692583602E-5</v>
       </c>
       <c r="M25" s="8">
-        <v>-2.70066441647624E-5</v>
+        <v>-2.7568287042084499E-5</v>
       </c>
       <c r="N25" s="8">
-        <v>-3.9139181867130601E-5</v>
+        <v>-3.5213531937796298E-5</v>
       </c>
       <c r="O25" s="8">
-        <v>-4.2169182807177201E-5</v>
+        <v>-3.1161916154452298E-5</v>
       </c>
       <c r="P25" s="8">
-        <v>-4.5730450361094003E-5</v>
+        <v>-3.8629289670829497E-5</v>
       </c>
       <c r="Q25" s="8">
-        <v>-1.6152441777825999E-5</v>
+        <v>-1.5899863080785099E-5</v>
       </c>
       <c r="R25" s="8">
-        <v>-2.11878228634332E-5</v>
+        <v>-1.3505716957335199E-5</v>
       </c>
       <c r="S25" s="8">
-        <v>-1.58810188010869E-5</v>
+        <v>-1.8053239998575698E-5</v>
       </c>
       <c r="T25" s="8">
-        <v>-2.0674534998908601E-5</v>
+        <v>-2.1045161391780598E-5</v>
       </c>
       <c r="U25" s="8">
-        <v>-1.61364046784057E-5</v>
+        <v>-1.5544439150787701E-5</v>
       </c>
       <c r="V25" s="8">
-        <v>-1.08559109154975E-5</v>
+        <v>-4.3231121222062101E-6</v>
       </c>
       <c r="W25" s="8">
-        <v>1.08416010636646E-5</v>
+        <v>8.1752607270381502E-6</v>
       </c>
       <c r="X25" s="8">
-        <v>1.4938019577859699E-6</v>
+        <v>2.7763091305072701E-6</v>
       </c>
       <c r="Y25" s="8">
-        <v>3.0427461575922E-5</v>
+        <v>1.0191418051885299E-5</v>
       </c>
       <c r="Z25" s="8">
-        <v>4.5558886692049198E-5</v>
+        <v>2.9097044136189399E-5</v>
       </c>
       <c r="AA25" s="8">
-        <v>-2.3157242354800602E-6</v>
+        <v>-1.1467170946729699E-6</v>
       </c>
       <c r="AB25" s="8">
-        <v>2.9363003382122201E-9</v>
+        <v>-4.2464853157679597E-9</v>
       </c>
       <c r="AC25" s="8">
-        <v>2.3578124301434599E-6</v>
+        <v>1.72407959539562E-6</v>
       </c>
       <c r="AD25" s="8">
-        <v>2.57254065320073E-8</v>
+        <v>-5.6509856825766598E-8</v>
       </c>
       <c r="AE25" s="8">
-        <v>6.1527968945627998E-6</v>
+        <v>1.16265602676479E-7</v>
       </c>
       <c r="AF25" s="8">
-        <v>-5.4770324948967097E-4</v>
+        <v>-3.1655779212900299E-4</v>
       </c>
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.25">
@@ -7222,97 +7223,97 @@
         <v>48</v>
       </c>
       <c r="B26" s="8">
-        <v>3.0835126259059799E-2</v>
+        <v>3.44833105647986E-2</v>
       </c>
       <c r="C26" s="8">
-        <v>4.9960856219291698E-5</v>
+        <v>3.8277125207519503E-5</v>
       </c>
       <c r="D26" s="8">
-        <v>-2.8996706449829501E-5</v>
+        <v>-2.26315833790098E-5</v>
       </c>
       <c r="E26" s="8">
-        <v>2.1523857111346501E-4</v>
+        <v>1.68765660797707E-4</v>
       </c>
       <c r="F26" s="8">
-        <v>2.8670363005618002E-5</v>
+        <v>2.2092207183286601E-5</v>
       </c>
       <c r="G26" s="8">
-        <v>-1.311447909988E-5</v>
+        <v>-3.2191950471297599E-6</v>
       </c>
       <c r="H26" s="8">
-        <v>2.2964596690976501E-5</v>
+        <v>1.36824618717904E-5</v>
       </c>
       <c r="I26" s="8">
-        <v>1.5377625981489099E-5</v>
+        <v>7.1549796684478098E-6</v>
       </c>
       <c r="J26" s="8">
-        <v>4.4795847847080399E-5</v>
+        <v>2.4342448627462001E-5</v>
       </c>
       <c r="K26" s="8">
-        <v>1.0765165245551999E-5</v>
+        <v>8.7678985060418204E-6</v>
       </c>
       <c r="L26" s="8">
-        <v>4.6770773274575097E-5</v>
+        <v>3.0784171367229803E-5</v>
       </c>
       <c r="M26" s="8">
-        <v>4.2996462274552398E-5</v>
+        <v>2.04241287357682E-5</v>
       </c>
       <c r="N26" s="8">
-        <v>4.8440801622610499E-5</v>
+        <v>3.1758192246236301E-5</v>
       </c>
       <c r="O26" s="8">
-        <v>4.0700433989505798E-5</v>
+        <v>3.0056493142876501E-5</v>
       </c>
       <c r="P26" s="8">
-        <v>4.9743362690267503E-5</v>
+        <v>3.4304687460243302E-5</v>
       </c>
       <c r="Q26" s="8">
-        <v>6.6962399651288395E-5</v>
+        <v>5.3283980456599201E-5</v>
       </c>
       <c r="R26" s="8">
-        <v>1.9688040213070699E-5</v>
+        <v>1.61817515153918E-5</v>
       </c>
       <c r="S26" s="8">
-        <v>2.6776318544249002E-5</v>
+        <v>1.8281612615116899E-5</v>
       </c>
       <c r="T26" s="8">
-        <v>3.8778006033768097E-5</v>
+        <v>4.3348141485591701E-5</v>
       </c>
       <c r="U26" s="8">
-        <v>5.8067607343704796E-6</v>
+        <v>-7.7485180559398298E-7</v>
       </c>
       <c r="V26" s="8">
-        <v>7.6812333750776906E-6</v>
+        <v>3.55431784952156E-6</v>
       </c>
       <c r="W26" s="8">
-        <v>4.9036715918067804E-6</v>
+        <v>-9.9580742348248902E-7</v>
       </c>
       <c r="X26" s="8">
-        <v>1.15262719514252E-5</v>
+        <v>3.7883514038165999E-6</v>
       </c>
       <c r="Y26" s="8">
-        <v>-1.13531822386823E-4</v>
+        <v>-9.3111197209676402E-5</v>
       </c>
       <c r="Z26" s="8">
-        <v>-2.3157242354800602E-6</v>
+        <v>-1.1467170946729699E-6</v>
       </c>
       <c r="AA26" s="8">
-        <v>4.4750718116636899E-5</v>
+        <v>3.2815396537098903E-5</v>
       </c>
       <c r="AB26" s="8">
-        <v>-4.1543863283167601E-7</v>
+        <v>-3.0795534846573098E-7</v>
       </c>
       <c r="AC26" s="8">
-        <v>-5.2217453214685201E-6</v>
+        <v>-3.80850560200112E-6</v>
       </c>
       <c r="AD26" s="8">
-        <v>-1.83850311204586E-6</v>
+        <v>-1.3507813705517501E-6</v>
       </c>
       <c r="AE26" s="8">
-        <v>1.9844403148915799E-5</v>
+        <v>1.3982340417995101E-5</v>
       </c>
       <c r="AF26" s="8">
-        <v>-1.00100479164715E-3</v>
+        <v>-7.28529333887984E-4</v>
       </c>
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.25">
@@ -7320,97 +7321,97 @@
         <v>49</v>
       </c>
       <c r="B27" s="8">
-        <v>-5.2935567153414298E-4</v>
+        <v>-5.5002444342896995E-4</v>
       </c>
       <c r="C27" s="8">
-        <v>-5.9271209308084304E-7</v>
+        <v>-4.4866372998640298E-7</v>
       </c>
       <c r="D27" s="8">
-        <v>1.4044594011223399E-7</v>
+        <v>1.12089594352502E-7</v>
       </c>
       <c r="E27" s="8">
-        <v>-1.8168299274073099E-6</v>
+        <v>-1.42675270740487E-6</v>
       </c>
       <c r="F27" s="8">
-        <v>-4.47720382063782E-7</v>
+        <v>-3.50618630472197E-7</v>
       </c>
       <c r="G27" s="8">
-        <v>7.7556325408841003E-8</v>
+        <v>-2.4461453760613501E-9</v>
       </c>
       <c r="H27" s="8">
-        <v>-4.59798533174453E-7</v>
+        <v>-3.2391900034712001E-7</v>
       </c>
       <c r="I27" s="8">
-        <v>-1.3942838193155E-7</v>
+        <v>-6.9358125359632595E-8</v>
       </c>
       <c r="J27" s="8">
-        <v>-3.5386117864702402E-7</v>
+        <v>-1.83799025828355E-7</v>
       </c>
       <c r="K27" s="8">
-        <v>-3.3441185155948299E-8</v>
+        <v>-4.4605772097792299E-8</v>
       </c>
       <c r="L27" s="8">
-        <v>-3.5225352668302998E-7</v>
+        <v>-2.32806765575063E-7</v>
       </c>
       <c r="M27" s="8">
-        <v>-3.2330155275160702E-7</v>
+        <v>-1.3118006608978299E-7</v>
       </c>
       <c r="N27" s="8">
-        <v>-4.1475301244220901E-7</v>
+        <v>-2.7943379093036902E-7</v>
       </c>
       <c r="O27" s="8">
-        <v>-3.5186698747759499E-7</v>
+        <v>-2.6997151693475101E-7</v>
       </c>
       <c r="P27" s="8">
-        <v>-3.9877838251645799E-7</v>
+        <v>-2.8371600823174798E-7</v>
       </c>
       <c r="Q27" s="8">
-        <v>-5.3591319747416199E-7</v>
+        <v>-4.2294495287388402E-7</v>
       </c>
       <c r="R27" s="8">
-        <v>-1.6705108955779699E-7</v>
+        <v>-1.4383094386253899E-7</v>
       </c>
       <c r="S27" s="8">
-        <v>-1.11104502723895E-7</v>
+        <v>-8.9271201703801602E-8</v>
       </c>
       <c r="T27" s="8">
-        <v>-2.1422466781597199E-7</v>
+        <v>-2.94314048158248E-7</v>
       </c>
       <c r="U27" s="8">
-        <v>1.6785398136138201E-8</v>
+        <v>5.8901365886500302E-8</v>
       </c>
       <c r="V27" s="8">
-        <v>8.5731017040313501E-9</v>
+        <v>2.5441536155777301E-8</v>
       </c>
       <c r="W27" s="8">
-        <v>4.1038573731187402E-8</v>
+        <v>7.8676433748307596E-8</v>
       </c>
       <c r="X27" s="8">
-        <v>-6.6715033595401904E-8</v>
+        <v>-1.3253464341926199E-9</v>
       </c>
       <c r="Y27" s="8">
-        <v>1.2905898832123601E-6</v>
+        <v>1.0366058796827001E-6</v>
       </c>
       <c r="Z27" s="8">
-        <v>2.9363003382122201E-9</v>
+        <v>-4.2464853157679597E-9</v>
       </c>
       <c r="AA27" s="8">
-        <v>-4.1543863283167601E-7</v>
+        <v>-3.0795534846573098E-7</v>
       </c>
       <c r="AB27" s="8">
-        <v>4.0323122486170099E-9</v>
+        <v>3.0299693811011099E-9</v>
       </c>
       <c r="AC27" s="8">
-        <v>5.4277559971531603E-8</v>
+        <v>4.0509506026858202E-8</v>
       </c>
       <c r="AD27" s="8">
-        <v>2.65223247507377E-8</v>
+        <v>1.9480536584234701E-8</v>
       </c>
       <c r="AE27" s="8">
-        <v>-2.13074029724394E-7</v>
+        <v>-1.48020859038985E-7</v>
       </c>
       <c r="AF27" s="8">
-        <v>8.6369103105185E-6</v>
+        <v>6.3447809961763403E-6</v>
       </c>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.25">
@@ -7418,97 +7419,97 @@
         <v>18</v>
       </c>
       <c r="B28" s="8">
-        <v>0.51583020859116102</v>
+        <v>0.51434771842252602</v>
       </c>
       <c r="C28" s="8">
-        <v>1.9537367433311E-7</v>
+        <v>-2.0624941559523401E-6</v>
       </c>
       <c r="D28" s="8">
-        <v>2.8337035697823298E-5</v>
+        <v>1.7858610406278699E-5</v>
       </c>
       <c r="E28" s="8">
-        <v>-1.84771376259494E-5</v>
+        <v>-1.3072422088211801E-5</v>
       </c>
       <c r="F28" s="8">
-        <v>-9.4755087277608297E-6</v>
+        <v>-9.7764234897121507E-6</v>
       </c>
       <c r="G28" s="8">
-        <v>3.2520195486707897E-5</v>
+        <v>2.1714595934536899E-5</v>
       </c>
       <c r="H28" s="8">
-        <v>2.7340167579836E-5</v>
+        <v>1.5800251116395101E-5</v>
       </c>
       <c r="I28" s="8">
-        <v>5.5429808852070404E-6</v>
+        <v>6.6583969087507302E-6</v>
       </c>
       <c r="J28" s="8">
-        <v>-3.9788094929477201E-5</v>
+        <v>-2.1884028565649699E-5</v>
       </c>
       <c r="K28" s="8">
-        <v>4.7111321309611003E-6</v>
+        <v>4.6831607499127103E-6</v>
       </c>
       <c r="L28" s="8">
-        <v>-2.2271571190318501E-5</v>
+        <v>-1.61945059632531E-5</v>
       </c>
       <c r="M28" s="8">
-        <v>-4.1565924680129503E-5</v>
+        <v>-2.7274544463754799E-5</v>
       </c>
       <c r="N28" s="8">
-        <v>-3.80510178376622E-5</v>
+        <v>-2.5921318177962599E-5</v>
       </c>
       <c r="O28" s="8">
-        <v>-3.0025605176261102E-5</v>
+        <v>-1.9356988529694E-5</v>
       </c>
       <c r="P28" s="8">
-        <v>-2.1946171195734E-5</v>
+        <v>-1.32486692496256E-5</v>
       </c>
       <c r="Q28" s="8">
-        <v>-2.5704786345445799E-5</v>
+        <v>-1.5305125523319501E-5</v>
       </c>
       <c r="R28" s="8">
-        <v>1.3967176173467299E-5</v>
+        <v>7.5524382012530103E-6</v>
       </c>
       <c r="S28" s="8">
-        <v>-1.9960511563682401E-5</v>
+        <v>-1.5751065671979301E-5</v>
       </c>
       <c r="T28" s="8">
-        <v>-3.18285968860809E-5</v>
+        <v>-1.9989521205405801E-5</v>
       </c>
       <c r="U28" s="8">
-        <v>-9.8318830310963701E-6</v>
+        <v>-6.2973314165602897E-6</v>
       </c>
       <c r="V28" s="8">
-        <v>-1.62687339521438E-6</v>
+        <v>-1.89745777961124E-6</v>
       </c>
       <c r="W28" s="8">
-        <v>-3.60192170009771E-6</v>
+        <v>-1.4038264992738799E-7</v>
       </c>
       <c r="X28" s="8">
-        <v>3.3672766714307099E-7</v>
+        <v>-7.9601118039708399E-9</v>
       </c>
       <c r="Y28" s="8">
-        <v>-8.7595251560827796E-5</v>
+        <v>-6.7511039266497305E-5</v>
       </c>
       <c r="Z28" s="8">
-        <v>2.3578124301434599E-6</v>
+        <v>1.72407959539562E-6</v>
       </c>
       <c r="AA28" s="8">
-        <v>-5.2217453214685201E-6</v>
+        <v>-3.80850560200112E-6</v>
       </c>
       <c r="AB28" s="8">
-        <v>5.4277559971531603E-8</v>
+        <v>4.0509506026858202E-8</v>
       </c>
       <c r="AC28" s="8">
-        <v>3.21450533562608E-5</v>
+        <v>2.38353223919609E-5</v>
       </c>
       <c r="AD28" s="8">
-        <v>2.4955615048827599E-6</v>
+        <v>1.6735431270951999E-6</v>
       </c>
       <c r="AE28" s="8">
-        <v>2.1395071352209302E-5</v>
+        <v>1.7616931975248201E-5</v>
       </c>
       <c r="AF28" s="8">
-        <v>-3.9822032602121601E-4</v>
+        <v>-2.8588874847273901E-4</v>
       </c>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.25">
@@ -7516,97 +7517,97 @@
         <v>50</v>
       </c>
       <c r="B29" s="8">
-        <v>-4.6495034593857697E-2</v>
+        <v>-4.8851595888663703E-2</v>
       </c>
       <c r="C29" s="8">
-        <v>-2.2478727004080199E-7</v>
+        <v>-9.5378344862199601E-8</v>
       </c>
       <c r="D29" s="8">
-        <v>-7.3764160587729402E-6</v>
+        <v>-5.1376684707118898E-6</v>
       </c>
       <c r="E29" s="8">
-        <v>-7.7207431865631299E-7</v>
+        <v>-5.4949633685124295E-7</v>
       </c>
       <c r="F29" s="8">
-        <v>3.8557142933592896E-6</v>
+        <v>3.3160001429759501E-6</v>
       </c>
       <c r="G29" s="8">
-        <v>6.8154745404337501E-6</v>
+        <v>5.0993407326699696E-6</v>
       </c>
       <c r="H29" s="8">
-        <v>8.6260049450565798E-6</v>
+        <v>7.1121667669341403E-6</v>
       </c>
       <c r="I29" s="8">
-        <v>-6.2674598652166803E-7</v>
+        <v>1.15372813028391E-6</v>
       </c>
       <c r="J29" s="8">
-        <v>-2.47507421196567E-6</v>
+        <v>-9.6443425739680201E-7</v>
       </c>
       <c r="K29" s="8">
-        <v>5.7162517755333003E-6</v>
+        <v>5.3646374898221998E-6</v>
       </c>
       <c r="L29" s="8">
-        <v>-1.78348677322715E-6</v>
+        <v>-9.71923573944943E-7</v>
       </c>
       <c r="M29" s="8">
-        <v>-2.6753411503209099E-6</v>
+        <v>-1.3377557896753101E-6</v>
       </c>
       <c r="N29" s="8">
-        <v>-3.6009848806514798E-6</v>
+        <v>-1.7770997084841599E-6</v>
       </c>
       <c r="O29" s="8">
-        <v>-6.0834902577431698E-6</v>
+        <v>-3.3297926801775999E-6</v>
       </c>
       <c r="P29" s="8">
-        <v>-1.7093373471616401E-6</v>
+        <v>-8.7502828710036599E-7</v>
       </c>
       <c r="Q29" s="8">
-        <v>-3.4711754374417602E-7</v>
+        <v>8.4653209894722195E-7</v>
       </c>
       <c r="R29" s="8">
-        <v>-3.74664897787857E-6</v>
+        <v>-2.0810114648482401E-6</v>
       </c>
       <c r="S29" s="8">
-        <v>1.18052823990489E-5</v>
+        <v>6.3442488630703199E-6</v>
       </c>
       <c r="T29" s="8">
-        <v>-6.4599382033204897E-6</v>
+        <v>-4.9519808537223396E-6</v>
       </c>
       <c r="U29" s="8">
-        <v>-3.29264052820027E-6</v>
+        <v>-1.1643442175534399E-6</v>
       </c>
       <c r="V29" s="8">
-        <v>-1.01962893170838E-6</v>
+        <v>3.5107206495501398E-7</v>
       </c>
       <c r="W29" s="8">
-        <v>-3.82554767037291E-6</v>
+        <v>-1.5246218719420099E-6</v>
       </c>
       <c r="X29" s="8">
-        <v>-7.67978569468998E-6</v>
+        <v>-4.1293388728434297E-6</v>
       </c>
       <c r="Y29" s="8">
-        <v>8.5997175046871295E-5</v>
+        <v>6.6298046674749102E-5</v>
       </c>
       <c r="Z29" s="8">
-        <v>2.57254065320073E-8</v>
+        <v>-5.6509856825766598E-8</v>
       </c>
       <c r="AA29" s="8">
-        <v>-1.83850311204586E-6</v>
+        <v>-1.3507813705517501E-6</v>
       </c>
       <c r="AB29" s="8">
-        <v>2.65223247507377E-8</v>
+        <v>1.9480536584234701E-8</v>
       </c>
       <c r="AC29" s="8">
-        <v>2.4955615048827599E-6</v>
+        <v>1.6735431270951999E-6</v>
       </c>
       <c r="AD29" s="8">
-        <v>4.6702428543630904E-6</v>
+        <v>3.5327792613185398E-6</v>
       </c>
       <c r="AE29" s="8">
-        <v>-3.4286663556683602E-6</v>
+        <v>-2.7442379982238601E-6</v>
       </c>
       <c r="AF29" s="8">
-        <v>-2.41321405609707E-4</v>
+        <v>-1.8190705973703699E-4</v>
       </c>
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.25">
@@ -7614,97 +7615,97 @@
         <v>4</v>
       </c>
       <c r="B30" s="8">
-        <v>-0.50649597296139603</v>
+        <v>-0.50382008485685903</v>
       </c>
       <c r="C30" s="8">
-        <v>3.4765388771384202E-5</v>
+        <v>3.56806776970703E-5</v>
       </c>
       <c r="D30" s="8">
-        <v>2.4381918286106602E-5</v>
+        <v>3.2141074307096401E-5</v>
       </c>
       <c r="E30" s="8">
-        <v>5.6212547344424101E-5</v>
+        <v>4.0434918179314501E-5</v>
       </c>
       <c r="F30" s="8">
-        <v>2.2053885031994599E-4</v>
+        <v>1.58240065566467E-4</v>
       </c>
       <c r="G30" s="8">
-        <v>-5.2204729394408401E-5</v>
+        <v>-3.59681661507263E-5</v>
       </c>
       <c r="H30" s="8">
-        <v>8.1975869074248398E-5</v>
+        <v>1.9493443158649301E-5</v>
       </c>
       <c r="I30" s="8">
-        <v>1.29370215620344E-4</v>
+        <v>9.4318092781603798E-5</v>
       </c>
       <c r="J30" s="8">
-        <v>1.5554310311606301E-4</v>
+        <v>1.2351654348261799E-4</v>
       </c>
       <c r="K30" s="8">
-        <v>1.04825224356768E-4</v>
+        <v>8.7184867609805801E-5</v>
       </c>
       <c r="L30" s="8">
-        <v>1.1226244316264E-4</v>
+        <v>1.08484040202177E-4</v>
       </c>
       <c r="M30" s="8">
-        <v>2.10789727162438E-4</v>
+        <v>1.5480723694247199E-4</v>
       </c>
       <c r="N30" s="8">
-        <v>1.7958724863632199E-4</v>
+        <v>1.6026663310050399E-4</v>
       </c>
       <c r="O30" s="8">
-        <v>1.0183127722180401E-4</v>
+        <v>9.9770514449259805E-5</v>
       </c>
       <c r="P30" s="8">
-        <v>1.6744977284978299E-4</v>
+        <v>1.4781598336841001E-4</v>
       </c>
       <c r="Q30" s="8">
-        <v>1.5264729666305299E-4</v>
+        <v>1.76127397211751E-4</v>
       </c>
       <c r="R30" s="8">
-        <v>5.7211024127117701E-5</v>
+        <v>9.7167713338926502E-5</v>
       </c>
       <c r="S30" s="8">
-        <v>-5.8696423875529303E-5</v>
+        <v>2.7037100275640499E-6</v>
       </c>
       <c r="T30" s="8">
-        <v>-8.0821919107185804E-6</v>
+        <v>2.9485886840635E-6</v>
       </c>
       <c r="U30" s="8">
-        <v>1.1429896866467399E-6</v>
+        <v>-3.09401121375623E-6</v>
       </c>
       <c r="V30" s="8">
-        <v>6.3597273331523601E-5</v>
+        <v>5.2607278529689499E-5</v>
       </c>
       <c r="W30" s="8">
-        <v>2.79940389253745E-5</v>
+        <v>-2.30135253225843E-6</v>
       </c>
       <c r="X30" s="8">
-        <v>-1.69638255491436E-5</v>
+        <v>-2.4996167309672399E-5</v>
       </c>
       <c r="Y30" s="8">
-        <v>-6.1995988585808299E-5</v>
+        <v>-5.02039356084404E-5</v>
       </c>
       <c r="Z30" s="8">
-        <v>6.1527968945627998E-6</v>
+        <v>1.16265602676479E-7</v>
       </c>
       <c r="AA30" s="8">
-        <v>1.9844403148915799E-5</v>
+        <v>1.3982340417995101E-5</v>
       </c>
       <c r="AB30" s="8">
-        <v>-2.13074029724394E-7</v>
+        <v>-1.48020859038985E-7</v>
       </c>
       <c r="AC30" s="8">
-        <v>2.1395071352209302E-5</v>
+        <v>1.7616931975248201E-5</v>
       </c>
       <c r="AD30" s="8">
-        <v>-3.4286663556683602E-6</v>
+        <v>-2.7442379982238601E-6</v>
       </c>
       <c r="AE30" s="8">
-        <v>1.4002109993245799E-3</v>
+        <v>1.0885576163336701E-3</v>
       </c>
       <c r="AF30" s="8">
-        <v>-1.3786224490977099E-3</v>
+        <v>-1.01083119587212E-3</v>
       </c>
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.25">
@@ -7712,97 +7713,97 @@
         <v>8</v>
       </c>
       <c r="B31" s="8">
-        <v>7.2480123278155597</v>
+        <v>7.5133035790918301</v>
       </c>
       <c r="C31" s="8">
-        <v>-2.4542698855680098E-3</v>
+        <v>-1.8331472171509999E-3</v>
       </c>
       <c r="D31" s="8">
-        <v>2.7313052606342701E-5</v>
+        <v>1.3314311295563701E-4</v>
       </c>
       <c r="E31" s="8">
-        <v>-6.9135954020958096E-3</v>
+        <v>-5.4429747032758297E-3</v>
       </c>
       <c r="F31" s="8">
-        <v>-1.2890159632446599E-3</v>
+        <v>-9.6146032241205097E-4</v>
       </c>
       <c r="G31" s="8">
-        <v>-1.3619116532863601E-3</v>
+        <v>-1.2169697293377901E-3</v>
       </c>
       <c r="H31" s="8">
-        <v>-2.9328679580843601E-3</v>
+        <v>-2.16736343368281E-3</v>
       </c>
       <c r="I31" s="8">
-        <v>-3.9674796296594204E-3</v>
+        <v>-2.9119904647221199E-3</v>
       </c>
       <c r="J31" s="8">
-        <v>-4.3283767875363704E-3</v>
+        <v>-3.0405545572973602E-3</v>
       </c>
       <c r="K31" s="8">
-        <v>-4.99602939742893E-3</v>
+        <v>-3.6637257779822902E-3</v>
       </c>
       <c r="L31" s="8">
-        <v>-4.7173784418936696E-3</v>
+        <v>-3.34205043482237E-3</v>
       </c>
       <c r="M31" s="8">
-        <v>-4.5881572585573698E-3</v>
+        <v>-3.0863304901270999E-3</v>
       </c>
       <c r="N31" s="8">
-        <v>-4.4290039680673597E-3</v>
+        <v>-3.1617315106646999E-3</v>
       </c>
       <c r="O31" s="8">
-        <v>-3.9710661631880704E-3</v>
+        <v>-3.04941863417782E-3</v>
       </c>
       <c r="P31" s="8">
-        <v>-4.7488306469483897E-3</v>
+        <v>-3.41639667813341E-3</v>
       </c>
       <c r="Q31" s="8">
-        <v>-5.6465546488757897E-3</v>
+        <v>-4.2994049611112502E-3</v>
       </c>
       <c r="R31" s="8">
-        <v>-4.2919591708235599E-3</v>
+        <v>-3.30926235510124E-3</v>
       </c>
       <c r="S31" s="8">
-        <v>-5.3557541859268901E-3</v>
+        <v>-3.6254356706759902E-3</v>
       </c>
       <c r="T31" s="8">
-        <v>-7.4725403196196198E-4</v>
+        <v>-8.2595513948921604E-4</v>
       </c>
       <c r="U31" s="8">
-        <v>-2.2103235855487598E-3</v>
+        <v>-1.41664342203662E-3</v>
       </c>
       <c r="V31" s="8">
-        <v>-2.8409735738362499E-3</v>
+        <v>-2.023016610261E-3</v>
       </c>
       <c r="W31" s="8">
-        <v>-3.08464000034487E-3</v>
+        <v>-2.1170347658758001E-3</v>
       </c>
       <c r="X31" s="8">
-        <v>-3.3052825074266099E-3</v>
+        <v>-2.3505563205864898E-3</v>
       </c>
       <c r="Y31" s="8">
-        <v>-2.86707906624437E-3</v>
+        <v>-1.7936134470325799E-3</v>
       </c>
       <c r="Z31" s="8">
-        <v>-5.4770324948967097E-4</v>
+        <v>-3.1655779212900299E-4</v>
       </c>
       <c r="AA31" s="8">
-        <v>-1.00100479164715E-3</v>
+        <v>-7.28529333887984E-4</v>
       </c>
       <c r="AB31" s="8">
-        <v>8.6369103105185E-6</v>
+        <v>6.3447809961763403E-6</v>
       </c>
       <c r="AC31" s="8">
-        <v>-3.9822032602121601E-4</v>
+        <v>-2.8588874847273901E-4</v>
       </c>
       <c r="AD31" s="8">
-        <v>-2.41321405609707E-4</v>
+        <v>-1.8190705973703699E-4</v>
       </c>
       <c r="AE31" s="8">
-        <v>-1.3786224490977099E-3</v>
+        <v>-1.01083119587212E-3</v>
       </c>
       <c r="AF31" s="8">
-        <v>6.2092217083099303E-2</v>
+        <v>4.3828008715741301E-2</v>
       </c>
     </row>
   </sheetData>
@@ -7812,14 +7813,15 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59539B72-1230-4A6D-80E6-59AE8E093E38}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39740585-ECE9-465B-B340-FC9F2AA7D554}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.42578125" style="8"/>
+    <col min="1" max="1" width="30.7109375" style="8" customWidth="1"/>
+    <col min="2" max="16384" width="11.42578125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -7859,10 +7861,10 @@
         <v>9</v>
       </c>
       <c r="B2" s="8">
-        <v>0.94648283319485504</v>
+        <v>2.2308687127043498</v>
       </c>
       <c r="C2" s="8">
-        <v>4.6046027090929101E-2</v>
+        <v>6.5940278412306597E-2</v>
       </c>
       <c r="D2" s="8">
         <v>0</v>
@@ -7891,13 +7893,13 @@
         <v>10</v>
       </c>
       <c r="B3" s="8">
-        <v>-0.74452787110320595</v>
+        <v>-0.30192581306493699</v>
       </c>
       <c r="C3" s="8">
         <v>0</v>
       </c>
       <c r="D3" s="8">
-        <v>3.8881675172174397E-2</v>
+        <v>7.5212452838669494E-2</v>
       </c>
       <c r="E3" s="8">
         <v>0</v>
@@ -7923,7 +7925,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="8">
-        <v>8.6643254685205701E-2</v>
+        <v>2.2472156436933899</v>
       </c>
       <c r="C4" s="8">
         <v>0</v>
@@ -7932,7 +7934,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="8">
-        <v>4.6383158344720898E-2</v>
+        <v>0.10969848117255999</v>
       </c>
       <c r="F4" s="8">
         <v>0</v>
@@ -7955,7 +7957,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="8">
-        <v>0.189027531625411</v>
+        <v>0.64869909269126902</v>
       </c>
       <c r="C5" s="8">
         <v>0</v>
@@ -7967,7 +7969,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="8">
-        <v>1.6809216722719799E-2</v>
+        <v>3.2433040660780399E-2</v>
       </c>
       <c r="G5" s="8">
         <v>0</v>
@@ -7987,7 +7989,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="8">
-        <v>0.170241292824688</v>
+        <v>0.247487279976882</v>
       </c>
       <c r="C6" s="8">
         <v>0</v>
@@ -8002,7 +8004,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="8">
-        <v>2.5361728500120799E-2</v>
+        <v>6.5649095772349397E-2</v>
       </c>
       <c r="H6" s="8">
         <v>0</v>
@@ -8019,7 +8021,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="8">
-        <v>0.48999654230929401</v>
+        <v>0.47342809895626298</v>
       </c>
       <c r="C7" s="8">
         <v>0</v>
@@ -8037,7 +8039,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="8">
-        <v>3.5297224625596098E-2</v>
+        <v>8.2853936821462401E-2</v>
       </c>
       <c r="I7" s="8">
         <v>0</v>
@@ -8051,7 +8053,7 @@
         <v>41</v>
       </c>
       <c r="B8" s="8">
-        <v>-6.3069856012254497E-2</v>
+        <v>0.115955640008294</v>
       </c>
       <c r="C8" s="8">
         <v>0</v>
@@ -8072,7 +8074,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="8">
-        <v>3.9868826801572697E-3</v>
+        <v>4.3199823340228701E-3</v>
       </c>
       <c r="J8" s="8">
         <v>0</v>
@@ -8083,7 +8085,7 @@
         <v>42</v>
       </c>
       <c r="B9" s="8">
-        <v>2.3857195384732799E-2</v>
+        <v>-4.5846181593811902E-2</v>
       </c>
       <c r="C9" s="8">
         <v>0</v>
@@ -8107,7 +8109,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="8">
-        <v>2.61799734934479E-3</v>
+        <v>5.5223831446959302E-3</v>
       </c>
     </row>
   </sheetData>
@@ -8117,14 +8119,15 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2117C167-BBBF-44E5-8FF1-972C53EC0081}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCCA8CDA-6B32-4591-B626-E528AD0FFA09}">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.42578125" style="8"/>
+    <col min="1" max="1" width="30.7109375" style="8" customWidth="1"/>
+    <col min="2" max="16384" width="11.42578125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -8164,10 +8167,10 @@
         <v>9</v>
       </c>
       <c r="B2" s="8">
-        <v>1.31222396910015</v>
+        <v>1.57794483170301</v>
       </c>
       <c r="C2" s="8">
-        <v>7.2415398598534603E-2</v>
+        <v>4.4525432283931202E-2</v>
       </c>
       <c r="D2" s="8">
         <v>0</v>
@@ -8196,13 +8199,13 @@
         <v>10</v>
       </c>
       <c r="B3" s="8">
-        <v>-0.83232884836702503</v>
+        <v>-0.44526296712864499</v>
       </c>
       <c r="C3" s="8">
         <v>0</v>
       </c>
       <c r="D3" s="8">
-        <v>6.1759597205023498E-2</v>
+        <v>3.1298488008007601E-2</v>
       </c>
       <c r="E3" s="8">
         <v>0</v>
@@ -8228,7 +8231,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="8">
-        <v>0.62385513389612701</v>
+        <v>0.95918422877926801</v>
       </c>
       <c r="C4" s="8">
         <v>0</v>
@@ -8237,7 +8240,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="8">
-        <v>9.7341686841387998E-2</v>
+        <v>4.0999388247078501E-2</v>
       </c>
       <c r="F4" s="8">
         <v>0</v>
@@ -8260,7 +8263,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="8">
-        <v>0.45165677214143501</v>
+        <v>0.410449201544345</v>
       </c>
       <c r="C5" s="8">
         <v>0</v>
@@ -8272,7 +8275,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="8">
-        <v>2.1906510584743601E-2</v>
+        <v>2.48672606982888E-2</v>
       </c>
       <c r="G5" s="8">
         <v>0</v>
@@ -8292,7 +8295,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="8">
-        <v>0.22555831414433999</v>
+        <v>0.51357839382913895</v>
       </c>
       <c r="C6" s="8">
         <v>0</v>
@@ -8307,7 +8310,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="8">
-        <v>3.5551707986293E-2</v>
+        <v>4.6688208376807899E-2</v>
       </c>
       <c r="H6" s="8">
         <v>0</v>
@@ -8324,7 +8327,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="8">
-        <v>0.56553085623078203</v>
+        <v>0.90797354812527298</v>
       </c>
       <c r="C7" s="8">
         <v>0</v>
@@ -8342,7 +8345,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="8">
-        <v>4.8305181175741001E-2</v>
+        <v>6.2768857792423097E-2</v>
       </c>
       <c r="I7" s="8">
         <v>0</v>
@@ -8356,7 +8359,7 @@
         <v>41</v>
       </c>
       <c r="B8" s="8">
-        <v>-9.1966775986940905E-2</v>
+        <v>6.9757710534505496E-2</v>
       </c>
       <c r="C8" s="8">
         <v>0</v>
@@ -8377,7 +8380,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="8">
-        <v>4.5653133504445203E-3</v>
+        <v>4.0833692655597303E-3</v>
       </c>
       <c r="J8" s="8">
         <v>0</v>
@@ -8388,7 +8391,7 @@
         <v>42</v>
       </c>
       <c r="B9" s="8">
-        <v>6.5276887391865102E-2</v>
+        <v>-7.9821077067514498E-2</v>
       </c>
       <c r="C9" s="8">
         <v>0</v>
@@ -8412,7 +8415,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="8">
-        <v>2.8592596903319698E-3</v>
+        <v>7.27123173416502E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>